<commit_message>
Sprint 2 Acceptance Test Plan
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -49,6 +49,7 @@
         <b val="1"/>
         <color theme="1"/>
         <sz val="12"/>
+        <scheme val="none"/>
       </rPr>
       <t xml:space="preserve"> 2231-swen-261-10-a Speedy Racers</t>
     </r>
@@ -123,6 +124,7 @@
         <b val="1"/>
         <color theme="1"/>
         <sz val="12"/>
+        <scheme val="none"/>
       </rPr>
       <t>u-fund</t>
     </r>
@@ -131,6 +133,7 @@
         <rFont val="Calibri"/>
         <color theme="1"/>
         <sz val="12"/>
+        <scheme val="none"/>
       </rPr>
       <t xml:space="preserve"> site when I am not on the </t>
     </r>
@@ -140,6 +143,7 @@
         <b val="1"/>
         <color theme="1"/>
         <sz val="12"/>
+        <scheme val="none"/>
       </rPr>
       <t>Needs</t>
     </r>
@@ -148,6 +152,7 @@
         <rFont val="Calibri"/>
         <color theme="1"/>
         <sz val="12"/>
+        <scheme val="none"/>
       </rPr>
       <t xml:space="preserve"> page then I must see a means to navigate to the </t>
     </r>
@@ -157,6 +162,7 @@
         <b val="1"/>
         <color theme="1"/>
         <sz val="12"/>
+        <scheme val="none"/>
       </rPr>
       <t>Needs</t>
     </r>
@@ -165,142 +171,20 @@
         <rFont val="Calibri"/>
         <color theme="1"/>
         <sz val="12"/>
+        <scheme val="none"/>
       </rPr>
       <t xml:space="preserve"> page.</t>
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Given that I am not on the </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t>Needs</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t xml:space="preserve"> page when I choose the </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t>Needs</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t xml:space="preserve"> page then I am taken to the </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t>Needs</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t xml:space="preserve"> page.</t>
-    </r>
+    <t>Pass</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Given that I am on the </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t>Needs</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t xml:space="preserve"> page when there are no </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t>needs</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t xml:space="preserve"> in the </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t>cupboard</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t xml:space="preserve"> I see a message indicating that that there are no </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t>needs</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t xml:space="preserve"> available to contribute.</t>
-    </r>
+    <t>A.M; 03/19/2025</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Given that I am on the </t>
+      <t xml:space="preserve">Given that I am not on the </t>
     </r>
     <r>
       <rPr>
@@ -308,6 +192,7 @@
         <b val="1"/>
         <color theme="1"/>
         <sz val="12"/>
+        <scheme val="none"/>
       </rPr>
       <t>Needs</t>
     </r>
@@ -316,8 +201,9 @@
         <rFont val="Calibri"/>
         <color theme="1"/>
         <sz val="12"/>
-      </rPr>
-      <t xml:space="preserve"> page when there are </t>
+        <scheme val="none"/>
+      </rPr>
+      <t xml:space="preserve"> page when I choose the </t>
     </r>
     <r>
       <rPr>
@@ -325,16 +211,18 @@
         <b val="1"/>
         <color theme="1"/>
         <sz val="12"/>
-      </rPr>
-      <t>needs</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t xml:space="preserve"> in the </t>
+        <scheme val="none"/>
+      </rPr>
+      <t>Needs</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t xml:space="preserve"> page then I am taken to the </t>
     </r>
     <r>
       <rPr>
@@ -342,33 +230,18 @@
         <b val="1"/>
         <color theme="1"/>
         <sz val="12"/>
-      </rPr>
-      <t>cupboard</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t xml:space="preserve"> then I see each </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t>need</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t xml:space="preserve"> and short description.</t>
+        <scheme val="none"/>
+      </rPr>
+      <t>Needs</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t xml:space="preserve"> page.</t>
     </r>
   </si>
   <si>
@@ -381,6 +254,7 @@
         <b val="1"/>
         <color theme="1"/>
         <sz val="12"/>
+        <scheme val="none"/>
       </rPr>
       <t>Needs</t>
     </r>
@@ -389,8 +263,9 @@
         <rFont val="Calibri"/>
         <color theme="1"/>
         <sz val="12"/>
-      </rPr>
-      <t xml:space="preserve"> page when there are </t>
+        <scheme val="none"/>
+      </rPr>
+      <t xml:space="preserve"> page when there are no </t>
     </r>
     <r>
       <rPr>
@@ -398,6 +273,7 @@
         <b val="1"/>
         <color theme="1"/>
         <sz val="12"/>
+        <scheme val="none"/>
       </rPr>
       <t>needs</t>
     </r>
@@ -406,6 +282,7 @@
         <rFont val="Calibri"/>
         <color theme="1"/>
         <sz val="12"/>
+        <scheme val="none"/>
       </rPr>
       <t xml:space="preserve"> in the </t>
     </r>
@@ -415,6 +292,7 @@
         <b val="1"/>
         <color theme="1"/>
         <sz val="12"/>
+        <scheme val="none"/>
       </rPr>
       <t>cupboard</t>
     </r>
@@ -423,8 +301,9 @@
         <rFont val="Calibri"/>
         <color theme="1"/>
         <sz val="12"/>
-      </rPr>
-      <t xml:space="preserve"> then I see a means to add each </t>
+        <scheme val="none"/>
+      </rPr>
+      <t xml:space="preserve"> I see a message indicating that that there are no </t>
     </r>
     <r>
       <rPr>
@@ -432,65 +311,255 @@
         <b val="1"/>
         <color theme="1"/>
         <sz val="12"/>
-      </rPr>
-      <t>need</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t xml:space="preserve"> to my funding </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t>basket</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-      </rPr>
-      <t>.</t>
+        <scheme val="none"/>
+      </rPr>
+      <t>needs</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t xml:space="preserve"> available to contribute.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Funding basket obscurity </t>
+    <t>A.M.; 03/19/2025</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Given that I am on the </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="1"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t>Needs</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t xml:space="preserve"> page when there are </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="1"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t>needs</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t xml:space="preserve"> in the </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="1"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t>cupboard</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t xml:space="preserve"> then I see each </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="1"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t>need</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t xml:space="preserve"> and short description.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Given that I am on the </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="1"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t>Needs</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t xml:space="preserve"> page when there are </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="1"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t>needs</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t xml:space="preserve"> in the </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="1"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t>cupboard</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t xml:space="preserve"> then I see a means to add each </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="1"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t>need</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t xml:space="preserve"> to my funding </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="1"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t>basket</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <scheme val="none"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>As a U-fund Manager, I should not have access to the contents of funding baskets so that funding privacy is maintained.</t>
   </si>
   <si>
     <t>Given I am logged in as a U-fund Manager, when I navigate the system, then I do not see any Helper's funding basket.</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>E.L; 03/19/2025;</t>
+    <t>E.L.; 03/19/2025;</t>
   </si>
   <si>
     <t>Given I try to access basket data directly, when I do so, then I receive an error or restricted access message.</t>
   </si>
   <si>
-    <t>Create admin account</t>
+    <t>As a U-fund Manager, I want to manage the needs stored in the needs cupboard so that I can ensure accurate and up-to-date information.</t>
   </si>
   <si>
-    <t>Given I am a U-fund Manager when I login then I have the username "admin"</t>
+    <t>Given I am logged in as a U-fund Manager, when I visit the needs cupboard, then I can see all the stored needs.</t>
   </si>
   <si>
-    <t>Given I am a U-fund Manager when I login then I have different permissions than a helper and only U-fund managers may use this account</t>
+    <t>E.Z.W. 03/19/2025;</t>
+  </si>
+  <si>
+    <t>Given I want to add a new need, when I enter the details and submit, then the need is saved to the cupboard.</t>
+  </si>
+  <si>
+    <t>Given I want to update a need, when I modify its details and save, then the cupboard reflects the changes.</t>
+  </si>
+  <si>
+    <t>Given I want to delete a need, when I confirm removal, **then **the need is no longer in the cupboard.</t>
+  </si>
+  <si>
+    <t>Given I log out and log back in, when I visit the cupboard, then all modifications persist.</t>
+  </si>
+  <si>
+    <t>S.L.; 03/19/2025</t>
+  </si>
+  <si>
+    <t>As a Helper, I want to add or remove needs from my funding basket so that I can manage what I plan to fund.</t>
+  </si>
+  <si>
+    <t>Given I am viewing a need, when I click "Add to Basket," then the need is saved to my basket.</t>
+  </si>
+  <si>
+    <t>Given a need is already in my basket, when I click "Remove," then it is removed from my basket.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -525,9 +594,20 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -955,7 +1035,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="C1" xSplit="2"/>
-      <selection pane="topRight" activeCell="D10" sqref="D10"/>
+      <selection pane="topRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -996,100 +1076,181 @@
       <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="E2" s="9"/>
     </row>
     <row r="3" ht="31.5">
       <c r="A3" s="10"/>
       <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="E3" s="9"/>
     </row>
     <row r="4" ht="47.25">
       <c r="A4" s="10"/>
       <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="E4" s="9"/>
     </row>
     <row r="5" ht="31.5">
       <c r="A5" s="10"/>
       <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="9"/>
+        <v>18</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="E5" s="9"/>
     </row>
     <row r="6" ht="31.5">
       <c r="A6" s="10"/>
       <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="9"/>
+        <v>19</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" ht="31.5">
+    <row r="7" ht="63">
       <c r="A7" s="11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E7" s="9"/>
     </row>
     <row r="8" ht="31.5">
       <c r="B8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" ht="31.5">
+    <row r="9" ht="78.75">
       <c r="A9" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" ht="47.25">
+    <row r="10" ht="31.5">
       <c r="B10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="9"/>
+        <v>27</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11">
-      <c r="C11" s="9"/>
+    <row r="11" ht="31.5">
+      <c r="B11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12">
-      <c r="C12" s="9"/>
+    <row r="12" ht="31.5">
+      <c r="B12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E12" s="9"/>
     </row>
-    <row r="13">
-      <c r="C13" s="9"/>
+    <row r="13" ht="31.5">
+      <c r="B13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="E13" s="9"/>
     </row>
-    <row r="14">
-      <c r="C14" s="9"/>
+    <row r="14" ht="63">
+      <c r="A14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="E14" s="9"/>
     </row>
-    <row r="15">
-      <c r="C15" s="9"/>
+    <row r="15" ht="31.5">
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="E15" s="9"/>
     </row>
     <row r="16">
@@ -3372,33 +3533,33 @@
       <c r="C585" s="9"/>
       <c r="E585" s="9"/>
     </row>
-    <row r="586">
-      <c r="C586" s="9"/>
-      <c r="E586" s="9"/>
-    </row>
-    <row r="587">
-      <c r="C587" s="9"/>
-      <c r="E587" s="9"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D587 F2:F587">
+  <conditionalFormatting sqref="D9:D585 F9:F585">
     <cfRule priority="1" stopIfTrue="1" dxfId="0" type="expression">
+      <formula>AND(ISBLANK(D9),C9="Pass")</formula>
+    </cfRule>
+    <cfRule priority="3" stopIfTrue="1" dxfId="1" type="expression">
+      <formula>AND(ISBLANK(D9),C9="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D8 F2:F8">
+    <cfRule priority="2" stopIfTrue="1" dxfId="0" type="expression">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
-    <cfRule priority="2" stopIfTrue="1" dxfId="1" type="expression">
+    <cfRule priority="4" stopIfTrue="1" dxfId="1" type="expression">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C587 E2:E587">
-    <cfRule priority="3" dxfId="2" type="cellIs" operator="equal">
+  <conditionalFormatting sqref="C2:C585 E2:E585">
+    <cfRule priority="5" dxfId="2" type="cellIs" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule priority="4" dxfId="3" type="cellIs" operator="equal">
+    <cfRule priority="6" dxfId="3" type="cellIs" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C587 E2:E587">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C585 E2:E585">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated acceptance test plan to include Sprint 3 stories
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -1,39 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\water\Favorites\team-project-2245-swen-261-04-6f\etc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\team-project-2245-swen-261-04-6f\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4D67DC-940F-47FB-809B-6462C350850E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6645" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
     <sheet name="Test Plan" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>Instructions</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter your team name as specified in the cell below. When doing cross-team acceptance testing, enter the name for the testing group._x000d_
-_x000d_
-Fill-in the Test Plan worksheet with all the remaining User Stories in your Product Backlog.  Since Product acceptance is from the perspective of the end-user, only add User Stories that pertain to the Owner or Buyer and do not include User Stories specifically for the REST API service (e.g. AS a developer...)._x000d_
-_x000d_
-As your user stories are refined, add the acceptance criteria for each user story. Use a separate worksheet to provide any specific test case data that the tester needs to use._x000d_
-_x000d_
-As tests are performed in each sprint, indicate Pass/Fail.  Note that there are separate columns for each sprint.  The tester should add initials and a date in the comments column. If the test failed, the tester is required to add additional information about the failure. The status cell will color code based on the test results. The comments cell will color code when a test result exists but no information is entered._x000d_
-_x000d_
-Save this test plan with a name formatted as "term-swen-261-sec-letter name", e.g. 2231-swen-261-10-a Speedy Racers.xslx._x000d_
-_x000d_
+    <t>Enter your team name as specified in the cell below. When doing cross-team acceptance testing, enter the name for the testing group._x000D_
+_x000D_
+Fill-in the Test Plan worksheet with all the remaining User Stories in your Product Backlog.  Since Product acceptance is from the perspective of the end-user, only add User Stories that pertain to the Owner or Buyer and do not include User Stories specifically for the REST API service (e.g. AS a developer...)._x000D_
+_x000D_
+As your user stories are refined, add the acceptance criteria for each user story. Use a separate worksheet to provide any specific test case data that the tester needs to use._x000D_
+_x000D_
+As tests are performed in each sprint, indicate Pass/Fail.  Note that there are separate columns for each sprint.  The tester should add initials and a date in the comments column. If the test failed, the tester is required to add additional information about the failure. The status cell will color code based on the test results. The comments cell will color code when a test result exists but no information is entered._x000D_
+_x000D_
+Save this test plan with a name formatted as "term-swen-261-sec-letter name", e.g. 2231-swen-261-10-a Speedy Racers.xslx._x000D_
+_x000D_
 Submit this file per the instructions specified for the sprint submissions and cross-team testing.</t>
   </si>
   <si>
@@ -45,11 +47,10 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve"> 2231-swen-261-10-a Speedy Racers</t>
     </r>
@@ -81,38 +82,232 @@
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
         <rFont val="Arial"/>
-        <b val="1"/>
+      </rPr>
+      <t>helper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
         <color rgb="FF333333"/>
-        <scheme val="none"/>
-      </rPr>
-      <t>helper</t>
-    </r>
-    <r>
-      <rPr>
         <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> I want to see a list of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
         <color rgb="FF333333"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> I want to see a list of </t>
-    </r>
-    <r>
-      <rPr>
         <rFont val="Arial"/>
-        <b val="1"/>
+      </rPr>
+      <t>needs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
         <color rgb="FF333333"/>
-        <scheme val="none"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> so that I choose what to contribute to.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Given that I am on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>u-fund</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> site when I am not on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Needs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> page then I must see a means to navigate to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Needs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> page.</t>
+    </r>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>A.M; 03/19/2025</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Given that I am not on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Needs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> page when I choose the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Needs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> page then I am taken to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Needs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Given that I am on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Needs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> page when there are no </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t>needs</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF333333"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> so that I choose what to contribute to.</t>
-    </r>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>cupboard</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> I see a message indicating that that there are no </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>needs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> available to contribute.</t>
+    </r>
+  </si>
+  <si>
+    <t>A.M.; 03/19/2025</t>
   </si>
   <si>
     <r>
@@ -120,391 +315,159 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t>u-fund</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> site when I am not on the </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t>Needs</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> page then I must see a means to navigate to the </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> page when there are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>needs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>cupboard</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> then I see each </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>need</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> and short description.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Given that I am on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t>Needs</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> page.</t>
-    </r>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>A.M; 03/19/2025</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Given that I am not on the </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t>Needs</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> page when I choose the </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t>Needs</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> page then I am taken to the </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t>Needs</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> page.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Given that I am on the </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t>Needs</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> page when there are no </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> page when there are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t>needs</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve"> in the </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t>cupboard</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> I see a message indicating that that there are no </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t>needs</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> available to contribute.</t>
-    </r>
-  </si>
-  <si>
-    <t>A.M.; 03/19/2025</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Given that I am on the </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t>Needs</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> page when there are </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t>needs</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> in the </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t>cupboard</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> then I see each </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> then I see a means to add each </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t>need</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> and short description.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Given that I am on the </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t>Needs</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> page when there are </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t>needs</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> in the </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t>cupboard</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t xml:space="preserve"> then I see a means to add each </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
-      </rPr>
-      <t>need</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve"> to my funding </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Calibri"/>
-        <b val="1"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t>basket</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="12"/>
-        <scheme val="none"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t>.</t>
     </r>
@@ -553,13 +516,34 @@
   </si>
   <si>
     <t>Given a need is already in my basket, when I click "Remove," then it is removed from my basket.</t>
+  </si>
+  <si>
+    <t>As a Helper I want to check out and fund my selected needs so that I can complete my contribution</t>
+  </si>
+  <si>
+    <t>Given I have needs in my basket, when I proceed to checkout, then I will see a summary of what I am funding</t>
+  </si>
+  <si>
+    <t>Given I confirm the checkout, when I complete the process, then my basket is cleared and the needs are marked as funded</t>
+  </si>
+  <si>
+    <t>Given I log out and log back in, when I visit my basket, then I see an empty basket after a successful checkout</t>
+  </si>
+  <si>
+    <t>As a user, I want to save my changes so that I don't have to restart every time I log back in</t>
+  </si>
+  <si>
+    <t>Given I change something as a user, when I log out then I expect my changes to be saved for when I log back in</t>
+  </si>
+  <si>
+    <t>not implemented yet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -599,15 +583,20 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -619,11 +608,21 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -668,14 +667,24 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -689,18 +698,16 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -709,10 +716,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -984,23 +991,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" style="2" customWidth="1"/>
-    <col min="2" max="2" width="106.875" customWidth="1"/>
+    <col min="2" max="2" width="106.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="283.5">
+    <row r="1" spans="1:2" ht="279" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1008,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1016,7 +1026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1026,19 +1036,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup r:id="rId1" orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F585"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane activePane="topRight" state="frozen" topLeftCell="C1" xSplit="2"/>
-      <selection pane="topRight" activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30" style="4" customWidth="1"/>
     <col min="2" max="2" width="60" style="4" customWidth="1"/>
@@ -1046,10 +1057,10 @@
     <col min="4" max="4" width="60" style="4" customWidth="1"/>
     <col min="5" max="5" width="9" style="4" customWidth="1"/>
     <col min="6" max="6" width="60" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="10.875" style="6"/>
+    <col min="7" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -1069,7 +1080,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" ht="44.25">
+    <row r="2" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
@@ -1084,7 +1095,7 @@
       </c>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" ht="31.5">
+    <row r="3" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
@@ -1097,7 +1108,7 @@
       </c>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" ht="47.25">
+    <row r="4" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="4" t="s">
         <v>16</v>
@@ -1110,7 +1121,7 @@
       </c>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" ht="31.5">
+    <row r="5" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="10"/>
       <c r="B5" s="4" t="s">
         <v>18</v>
@@ -1123,7 +1134,7 @@
       </c>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" ht="31.5">
+    <row r="6" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="10"/>
       <c r="B6" s="4" t="s">
         <v>19</v>
@@ -1136,7 +1147,7 @@
       </c>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" ht="63">
+    <row r="7" spans="1:6" ht="62" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>20</v>
       </c>
@@ -1151,7 +1162,7 @@
       </c>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" ht="31.5">
+    <row r="8" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>23</v>
       </c>
@@ -1163,7 +1174,7 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" ht="78.75">
+    <row r="9" spans="1:6" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
@@ -1178,7 +1189,7 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" ht="31.5">
+    <row r="10" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1190,7 +1201,7 @@
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" ht="31.5">
+    <row r="11" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
@@ -1202,7 +1213,7 @@
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" ht="31.5">
+    <row r="12" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
@@ -1214,7 +1225,7 @@
       </c>
       <c r="E12" s="9"/>
     </row>
-    <row r="13" ht="31.5">
+    <row r="13" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
         <v>30</v>
       </c>
@@ -1226,7 +1237,7 @@
       </c>
       <c r="E13" s="9"/>
     </row>
-    <row r="14" ht="63">
+    <row r="14" spans="1:6" ht="62" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -1241,7 +1252,7 @@
       </c>
       <c r="E14" s="9"/>
     </row>
-    <row r="15" ht="31.5">
+    <row r="15" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>34</v>
       </c>
@@ -1253,2317 +1264,2339 @@
       </c>
       <c r="E15" s="9"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="C16" s="9"/>
+      <c r="D16" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="E16" s="9"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="B17" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="C17" s="9"/>
+      <c r="D17" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="E17" s="9"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="B18" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="C18" s="9"/>
+      <c r="D18" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="E18" s="9"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C19" s="9"/>
+      <c r="D19" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="E19" s="9"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C20" s="9"/>
       <c r="E20" s="9"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C21" s="9"/>
       <c r="E21" s="9"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C22" s="9"/>
       <c r="E22" s="9"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C23" s="9"/>
       <c r="E23" s="9"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
       <c r="E24" s="9"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
       <c r="E25" s="9"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C26" s="9"/>
       <c r="E26" s="9"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C27" s="9"/>
       <c r="E27" s="9"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C28" s="9"/>
       <c r="E28" s="9"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C29" s="9"/>
       <c r="E29" s="9"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C30" s="9"/>
       <c r="E30" s="9"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C31" s="9"/>
       <c r="E31" s="9"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C32" s="9"/>
       <c r="E32" s="9"/>
     </row>
-    <row r="33">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C33" s="9"/>
       <c r="E33" s="9"/>
     </row>
-    <row r="34">
+    <row r="34" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C34" s="9"/>
       <c r="E34" s="9"/>
     </row>
-    <row r="35">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C35" s="9"/>
       <c r="E35" s="9"/>
     </row>
-    <row r="36">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C36" s="9"/>
       <c r="E36" s="9"/>
     </row>
-    <row r="37">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C37" s="9"/>
       <c r="E37" s="9"/>
     </row>
-    <row r="38">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C38" s="9"/>
       <c r="E38" s="9"/>
     </row>
-    <row r="39">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C39" s="9"/>
       <c r="E39" s="9"/>
     </row>
-    <row r="40">
+    <row r="40" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C40" s="9"/>
       <c r="E40" s="9"/>
     </row>
-    <row r="41">
+    <row r="41" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C41" s="9"/>
       <c r="E41" s="9"/>
     </row>
-    <row r="42">
+    <row r="42" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C42" s="9"/>
       <c r="E42" s="9"/>
     </row>
-    <row r="43">
+    <row r="43" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C43" s="9"/>
       <c r="E43" s="9"/>
     </row>
-    <row r="44">
+    <row r="44" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C44" s="9"/>
       <c r="E44" s="9"/>
     </row>
-    <row r="45">
+    <row r="45" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C45" s="9"/>
       <c r="E45" s="9"/>
     </row>
-    <row r="46">
+    <row r="46" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C46" s="9"/>
       <c r="E46" s="9"/>
     </row>
-    <row r="47">
+    <row r="47" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C47" s="9"/>
       <c r="E47" s="9"/>
     </row>
-    <row r="48">
+    <row r="48" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C48" s="9"/>
       <c r="E48" s="9"/>
     </row>
-    <row r="49">
+    <row r="49" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C49" s="9"/>
       <c r="E49" s="9"/>
     </row>
-    <row r="50">
+    <row r="50" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C50" s="9"/>
       <c r="E50" s="9"/>
     </row>
-    <row r="51">
+    <row r="51" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C51" s="9"/>
       <c r="E51" s="9"/>
     </row>
-    <row r="52">
+    <row r="52" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C52" s="9"/>
       <c r="E52" s="9"/>
     </row>
-    <row r="53">
+    <row r="53" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C53" s="9"/>
       <c r="E53" s="9"/>
     </row>
-    <row r="54">
+    <row r="54" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C54" s="9"/>
       <c r="E54" s="9"/>
     </row>
-    <row r="55">
+    <row r="55" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C55" s="9"/>
       <c r="E55" s="9"/>
     </row>
-    <row r="56">
+    <row r="56" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C56" s="9"/>
       <c r="E56" s="9"/>
     </row>
-    <row r="57">
+    <row r="57" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C57" s="9"/>
       <c r="E57" s="9"/>
     </row>
-    <row r="58">
+    <row r="58" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C58" s="9"/>
       <c r="E58" s="9"/>
     </row>
-    <row r="59">
+    <row r="59" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C59" s="9"/>
       <c r="E59" s="9"/>
     </row>
-    <row r="60">
+    <row r="60" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C60" s="9"/>
       <c r="E60" s="9"/>
     </row>
-    <row r="61">
+    <row r="61" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C61" s="9"/>
       <c r="E61" s="9"/>
     </row>
-    <row r="62">
+    <row r="62" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C62" s="9"/>
       <c r="E62" s="9"/>
     </row>
-    <row r="63">
+    <row r="63" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C63" s="9"/>
       <c r="E63" s="9"/>
     </row>
-    <row r="64">
+    <row r="64" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C64" s="9"/>
       <c r="E64" s="9"/>
     </row>
-    <row r="65">
+    <row r="65" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C65" s="9"/>
       <c r="E65" s="9"/>
     </row>
-    <row r="66">
+    <row r="66" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C66" s="9"/>
       <c r="E66" s="9"/>
     </row>
-    <row r="67">
+    <row r="67" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C67" s="9"/>
       <c r="E67" s="9"/>
     </row>
-    <row r="68">
+    <row r="68" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C68" s="9"/>
       <c r="E68" s="9"/>
     </row>
-    <row r="69">
+    <row r="69" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C69" s="9"/>
       <c r="E69" s="9"/>
     </row>
-    <row r="70">
+    <row r="70" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C70" s="9"/>
       <c r="E70" s="9"/>
     </row>
-    <row r="71">
+    <row r="71" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C71" s="9"/>
       <c r="E71" s="9"/>
     </row>
-    <row r="72">
+    <row r="72" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C72" s="9"/>
       <c r="E72" s="9"/>
     </row>
-    <row r="73">
+    <row r="73" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C73" s="9"/>
       <c r="E73" s="9"/>
     </row>
-    <row r="74">
+    <row r="74" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C74" s="9"/>
       <c r="E74" s="9"/>
     </row>
-    <row r="75">
+    <row r="75" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C75" s="9"/>
       <c r="E75" s="9"/>
     </row>
-    <row r="76">
+    <row r="76" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C76" s="9"/>
       <c r="E76" s="9"/>
     </row>
-    <row r="77">
+    <row r="77" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C77" s="9"/>
       <c r="E77" s="9"/>
     </row>
-    <row r="78">
+    <row r="78" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C78" s="9"/>
       <c r="E78" s="9"/>
     </row>
-    <row r="79">
+    <row r="79" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C79" s="9"/>
       <c r="E79" s="9"/>
     </row>
-    <row r="80">
+    <row r="80" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C80" s="9"/>
       <c r="E80" s="9"/>
     </row>
-    <row r="81">
+    <row r="81" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C81" s="9"/>
       <c r="E81" s="9"/>
     </row>
-    <row r="82">
+    <row r="82" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C82" s="9"/>
       <c r="E82" s="9"/>
     </row>
-    <row r="83">
+    <row r="83" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C83" s="9"/>
       <c r="E83" s="9"/>
     </row>
-    <row r="84">
+    <row r="84" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C84" s="9"/>
       <c r="E84" s="9"/>
     </row>
-    <row r="85">
+    <row r="85" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C85" s="9"/>
       <c r="E85" s="9"/>
     </row>
-    <row r="86">
+    <row r="86" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C86" s="9"/>
       <c r="E86" s="9"/>
     </row>
-    <row r="87">
+    <row r="87" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C87" s="9"/>
       <c r="E87" s="9"/>
     </row>
-    <row r="88">
+    <row r="88" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C88" s="9"/>
       <c r="E88" s="9"/>
     </row>
-    <row r="89">
+    <row r="89" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C89" s="9"/>
       <c r="E89" s="9"/>
     </row>
-    <row r="90">
+    <row r="90" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C90" s="9"/>
       <c r="E90" s="9"/>
     </row>
-    <row r="91">
+    <row r="91" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C91" s="9"/>
       <c r="E91" s="9"/>
     </row>
-    <row r="92">
+    <row r="92" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C92" s="9"/>
       <c r="E92" s="9"/>
     </row>
-    <row r="93">
+    <row r="93" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C93" s="9"/>
       <c r="E93" s="9"/>
     </row>
-    <row r="94">
+    <row r="94" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C94" s="9"/>
       <c r="E94" s="9"/>
     </row>
-    <row r="95">
+    <row r="95" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C95" s="9"/>
       <c r="E95" s="9"/>
     </row>
-    <row r="96">
+    <row r="96" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C96" s="9"/>
       <c r="E96" s="9"/>
     </row>
-    <row r="97">
+    <row r="97" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C97" s="9"/>
       <c r="E97" s="9"/>
     </row>
-    <row r="98">
+    <row r="98" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C98" s="9"/>
       <c r="E98" s="9"/>
     </row>
-    <row r="99">
+    <row r="99" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C99" s="9"/>
       <c r="E99" s="9"/>
     </row>
-    <row r="100">
+    <row r="100" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C100" s="9"/>
       <c r="E100" s="9"/>
     </row>
-    <row r="101">
+    <row r="101" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C101" s="9"/>
       <c r="E101" s="9"/>
     </row>
-    <row r="102">
+    <row r="102" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C102" s="9"/>
       <c r="E102" s="9"/>
     </row>
-    <row r="103">
+    <row r="103" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C103" s="9"/>
       <c r="E103" s="9"/>
     </row>
-    <row r="104">
+    <row r="104" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C104" s="9"/>
       <c r="E104" s="9"/>
     </row>
-    <row r="105">
+    <row r="105" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C105" s="9"/>
       <c r="E105" s="9"/>
     </row>
-    <row r="106">
+    <row r="106" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C106" s="9"/>
       <c r="E106" s="9"/>
     </row>
-    <row r="107">
+    <row r="107" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C107" s="9"/>
       <c r="E107" s="9"/>
     </row>
-    <row r="108">
+    <row r="108" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C108" s="9"/>
       <c r="E108" s="9"/>
     </row>
-    <row r="109">
+    <row r="109" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C109" s="9"/>
       <c r="E109" s="9"/>
     </row>
-    <row r="110">
+    <row r="110" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C110" s="9"/>
       <c r="E110" s="9"/>
     </row>
-    <row r="111">
+    <row r="111" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C111" s="9"/>
       <c r="E111" s="9"/>
     </row>
-    <row r="112">
+    <row r="112" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C112" s="9"/>
       <c r="E112" s="9"/>
     </row>
-    <row r="113">
+    <row r="113" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C113" s="9"/>
       <c r="E113" s="9"/>
     </row>
-    <row r="114">
+    <row r="114" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C114" s="9"/>
       <c r="E114" s="9"/>
     </row>
-    <row r="115">
+    <row r="115" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C115" s="9"/>
       <c r="E115" s="9"/>
     </row>
-    <row r="116">
+    <row r="116" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C116" s="9"/>
       <c r="E116" s="9"/>
     </row>
-    <row r="117">
+    <row r="117" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C117" s="9"/>
       <c r="E117" s="9"/>
     </row>
-    <row r="118">
+    <row r="118" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C118" s="9"/>
       <c r="E118" s="9"/>
     </row>
-    <row r="119">
+    <row r="119" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C119" s="9"/>
       <c r="E119" s="9"/>
     </row>
-    <row r="120">
+    <row r="120" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C120" s="9"/>
       <c r="E120" s="9"/>
     </row>
-    <row r="121">
+    <row r="121" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C121" s="9"/>
       <c r="E121" s="9"/>
     </row>
-    <row r="122">
+    <row r="122" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C122" s="9"/>
       <c r="E122" s="9"/>
     </row>
-    <row r="123">
+    <row r="123" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C123" s="9"/>
       <c r="E123" s="9"/>
     </row>
-    <row r="124">
+    <row r="124" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C124" s="9"/>
       <c r="E124" s="9"/>
     </row>
-    <row r="125">
+    <row r="125" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C125" s="9"/>
       <c r="E125" s="9"/>
     </row>
-    <row r="126">
+    <row r="126" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C126" s="9"/>
       <c r="E126" s="9"/>
     </row>
-    <row r="127">
+    <row r="127" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C127" s="9"/>
       <c r="E127" s="9"/>
     </row>
-    <row r="128">
+    <row r="128" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C128" s="9"/>
       <c r="E128" s="9"/>
     </row>
-    <row r="129">
+    <row r="129" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C129" s="9"/>
       <c r="E129" s="9"/>
     </row>
-    <row r="130">
+    <row r="130" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C130" s="9"/>
       <c r="E130" s="9"/>
     </row>
-    <row r="131">
+    <row r="131" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C131" s="9"/>
       <c r="E131" s="9"/>
     </row>
-    <row r="132">
+    <row r="132" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C132" s="9"/>
       <c r="E132" s="9"/>
     </row>
-    <row r="133">
+    <row r="133" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C133" s="9"/>
       <c r="E133" s="9"/>
     </row>
-    <row r="134">
+    <row r="134" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C134" s="9"/>
       <c r="E134" s="9"/>
     </row>
-    <row r="135">
+    <row r="135" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C135" s="9"/>
       <c r="E135" s="9"/>
     </row>
-    <row r="136">
+    <row r="136" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C136" s="9"/>
       <c r="E136" s="9"/>
     </row>
-    <row r="137">
+    <row r="137" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C137" s="9"/>
       <c r="E137" s="9"/>
     </row>
-    <row r="138">
+    <row r="138" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C138" s="9"/>
       <c r="E138" s="9"/>
     </row>
-    <row r="139">
+    <row r="139" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C139" s="9"/>
       <c r="E139" s="9"/>
     </row>
-    <row r="140">
+    <row r="140" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C140" s="9"/>
       <c r="E140" s="9"/>
     </row>
-    <row r="141">
+    <row r="141" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C141" s="9"/>
       <c r="E141" s="9"/>
     </row>
-    <row r="142">
+    <row r="142" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C142" s="9"/>
       <c r="E142" s="9"/>
     </row>
-    <row r="143">
+    <row r="143" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C143" s="9"/>
       <c r="E143" s="9"/>
     </row>
-    <row r="144">
+    <row r="144" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C144" s="9"/>
       <c r="E144" s="9"/>
     </row>
-    <row r="145">
+    <row r="145" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C145" s="9"/>
       <c r="E145" s="9"/>
     </row>
-    <row r="146">
+    <row r="146" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C146" s="9"/>
       <c r="E146" s="9"/>
     </row>
-    <row r="147">
+    <row r="147" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C147" s="9"/>
       <c r="E147" s="9"/>
     </row>
-    <row r="148">
+    <row r="148" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C148" s="9"/>
       <c r="E148" s="9"/>
     </row>
-    <row r="149">
+    <row r="149" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C149" s="9"/>
       <c r="E149" s="9"/>
     </row>
-    <row r="150">
+    <row r="150" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C150" s="9"/>
       <c r="E150" s="9"/>
     </row>
-    <row r="151">
+    <row r="151" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C151" s="9"/>
       <c r="E151" s="9"/>
     </row>
-    <row r="152">
+    <row r="152" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C152" s="9"/>
       <c r="E152" s="9"/>
     </row>
-    <row r="153">
+    <row r="153" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C153" s="9"/>
       <c r="E153" s="9"/>
     </row>
-    <row r="154">
+    <row r="154" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C154" s="9"/>
       <c r="E154" s="9"/>
     </row>
-    <row r="155">
+    <row r="155" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C155" s="9"/>
       <c r="E155" s="9"/>
     </row>
-    <row r="156">
+    <row r="156" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C156" s="9"/>
       <c r="E156" s="9"/>
     </row>
-    <row r="157">
+    <row r="157" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C157" s="9"/>
       <c r="E157" s="9"/>
     </row>
-    <row r="158">
+    <row r="158" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C158" s="9"/>
       <c r="E158" s="9"/>
     </row>
-    <row r="159">
+    <row r="159" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C159" s="9"/>
       <c r="E159" s="9"/>
     </row>
-    <row r="160">
+    <row r="160" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C160" s="9"/>
       <c r="E160" s="9"/>
     </row>
-    <row r="161">
+    <row r="161" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C161" s="9"/>
       <c r="E161" s="9"/>
     </row>
-    <row r="162">
+    <row r="162" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C162" s="9"/>
       <c r="E162" s="9"/>
     </row>
-    <row r="163">
+    <row r="163" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C163" s="9"/>
       <c r="E163" s="9"/>
     </row>
-    <row r="164">
+    <row r="164" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C164" s="9"/>
       <c r="E164" s="9"/>
     </row>
-    <row r="165">
+    <row r="165" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C165" s="9"/>
       <c r="E165" s="9"/>
     </row>
-    <row r="166">
+    <row r="166" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C166" s="9"/>
       <c r="E166" s="9"/>
     </row>
-    <row r="167">
+    <row r="167" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C167" s="9"/>
       <c r="E167" s="9"/>
     </row>
-    <row r="168">
+    <row r="168" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C168" s="9"/>
       <c r="E168" s="9"/>
     </row>
-    <row r="169">
+    <row r="169" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C169" s="9"/>
       <c r="E169" s="9"/>
     </row>
-    <row r="170">
+    <row r="170" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C170" s="9"/>
       <c r="E170" s="9"/>
     </row>
-    <row r="171">
+    <row r="171" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C171" s="9"/>
       <c r="E171" s="9"/>
     </row>
-    <row r="172">
+    <row r="172" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C172" s="9"/>
       <c r="E172" s="9"/>
     </row>
-    <row r="173">
+    <row r="173" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C173" s="9"/>
       <c r="E173" s="9"/>
     </row>
-    <row r="174">
+    <row r="174" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C174" s="9"/>
       <c r="E174" s="9"/>
     </row>
-    <row r="175">
+    <row r="175" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C175" s="9"/>
       <c r="E175" s="9"/>
     </row>
-    <row r="176">
+    <row r="176" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C176" s="9"/>
       <c r="E176" s="9"/>
     </row>
-    <row r="177">
+    <row r="177" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C177" s="9"/>
       <c r="E177" s="9"/>
     </row>
-    <row r="178">
+    <row r="178" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C178" s="9"/>
       <c r="E178" s="9"/>
     </row>
-    <row r="179">
+    <row r="179" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C179" s="9"/>
       <c r="E179" s="9"/>
     </row>
-    <row r="180">
+    <row r="180" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C180" s="9"/>
       <c r="E180" s="9"/>
     </row>
-    <row r="181">
+    <row r="181" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C181" s="9"/>
       <c r="E181" s="9"/>
     </row>
-    <row r="182">
+    <row r="182" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C182" s="9"/>
       <c r="E182" s="9"/>
     </row>
-    <row r="183">
+    <row r="183" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C183" s="9"/>
       <c r="E183" s="9"/>
     </row>
-    <row r="184">
+    <row r="184" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C184" s="9"/>
       <c r="E184" s="9"/>
     </row>
-    <row r="185">
+    <row r="185" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C185" s="9"/>
       <c r="E185" s="9"/>
     </row>
-    <row r="186">
+    <row r="186" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C186" s="9"/>
       <c r="E186" s="9"/>
     </row>
-    <row r="187">
+    <row r="187" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C187" s="9"/>
       <c r="E187" s="9"/>
     </row>
-    <row r="188">
+    <row r="188" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C188" s="9"/>
       <c r="E188" s="9"/>
     </row>
-    <row r="189">
+    <row r="189" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C189" s="9"/>
       <c r="E189" s="9"/>
     </row>
-    <row r="190">
+    <row r="190" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C190" s="9"/>
       <c r="E190" s="9"/>
     </row>
-    <row r="191">
+    <row r="191" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C191" s="9"/>
       <c r="E191" s="9"/>
     </row>
-    <row r="192">
+    <row r="192" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C192" s="9"/>
       <c r="E192" s="9"/>
     </row>
-    <row r="193">
+    <row r="193" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C193" s="9"/>
       <c r="E193" s="9"/>
     </row>
-    <row r="194">
+    <row r="194" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C194" s="9"/>
       <c r="E194" s="9"/>
     </row>
-    <row r="195">
+    <row r="195" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C195" s="9"/>
       <c r="E195" s="9"/>
     </row>
-    <row r="196">
+    <row r="196" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C196" s="9"/>
       <c r="E196" s="9"/>
     </row>
-    <row r="197">
+    <row r="197" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C197" s="9"/>
       <c r="E197" s="9"/>
     </row>
-    <row r="198">
+    <row r="198" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C198" s="9"/>
       <c r="E198" s="9"/>
     </row>
-    <row r="199">
+    <row r="199" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C199" s="9"/>
       <c r="E199" s="9"/>
     </row>
-    <row r="200">
+    <row r="200" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C200" s="9"/>
       <c r="E200" s="9"/>
     </row>
-    <row r="201">
+    <row r="201" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C201" s="9"/>
       <c r="E201" s="9"/>
     </row>
-    <row r="202">
+    <row r="202" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C202" s="9"/>
       <c r="E202" s="9"/>
     </row>
-    <row r="203">
+    <row r="203" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C203" s="9"/>
       <c r="E203" s="9"/>
     </row>
-    <row r="204">
+    <row r="204" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C204" s="9"/>
       <c r="E204" s="9"/>
     </row>
-    <row r="205">
+    <row r="205" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C205" s="9"/>
       <c r="E205" s="9"/>
     </row>
-    <row r="206">
+    <row r="206" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C206" s="9"/>
       <c r="E206" s="9"/>
     </row>
-    <row r="207">
+    <row r="207" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C207" s="9"/>
       <c r="E207" s="9"/>
     </row>
-    <row r="208">
+    <row r="208" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C208" s="9"/>
       <c r="E208" s="9"/>
     </row>
-    <row r="209">
+    <row r="209" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C209" s="9"/>
       <c r="E209" s="9"/>
     </row>
-    <row r="210">
+    <row r="210" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C210" s="9"/>
       <c r="E210" s="9"/>
     </row>
-    <row r="211">
+    <row r="211" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C211" s="9"/>
       <c r="E211" s="9"/>
     </row>
-    <row r="212">
+    <row r="212" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C212" s="9"/>
       <c r="E212" s="9"/>
     </row>
-    <row r="213">
+    <row r="213" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C213" s="9"/>
       <c r="E213" s="9"/>
     </row>
-    <row r="214">
+    <row r="214" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C214" s="9"/>
       <c r="E214" s="9"/>
     </row>
-    <row r="215">
+    <row r="215" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C215" s="9"/>
       <c r="E215" s="9"/>
     </row>
-    <row r="216">
+    <row r="216" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C216" s="9"/>
       <c r="E216" s="9"/>
     </row>
-    <row r="217">
+    <row r="217" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C217" s="9"/>
       <c r="E217" s="9"/>
     </row>
-    <row r="218">
+    <row r="218" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C218" s="9"/>
       <c r="E218" s="9"/>
     </row>
-    <row r="219">
+    <row r="219" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C219" s="9"/>
       <c r="E219" s="9"/>
     </row>
-    <row r="220">
+    <row r="220" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C220" s="9"/>
       <c r="E220" s="9"/>
     </row>
-    <row r="221">
+    <row r="221" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C221" s="9"/>
       <c r="E221" s="9"/>
     </row>
-    <row r="222">
+    <row r="222" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C222" s="9"/>
       <c r="E222" s="9"/>
     </row>
-    <row r="223">
+    <row r="223" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C223" s="9"/>
       <c r="E223" s="9"/>
     </row>
-    <row r="224">
+    <row r="224" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C224" s="9"/>
       <c r="E224" s="9"/>
     </row>
-    <row r="225">
+    <row r="225" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C225" s="9"/>
       <c r="E225" s="9"/>
     </row>
-    <row r="226">
+    <row r="226" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C226" s="9"/>
       <c r="E226" s="9"/>
     </row>
-    <row r="227">
+    <row r="227" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C227" s="9"/>
       <c r="E227" s="9"/>
     </row>
-    <row r="228">
+    <row r="228" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C228" s="9"/>
       <c r="E228" s="9"/>
     </row>
-    <row r="229">
+    <row r="229" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C229" s="9"/>
       <c r="E229" s="9"/>
     </row>
-    <row r="230">
+    <row r="230" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C230" s="9"/>
       <c r="E230" s="9"/>
     </row>
-    <row r="231">
+    <row r="231" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C231" s="9"/>
       <c r="E231" s="9"/>
     </row>
-    <row r="232">
+    <row r="232" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C232" s="9"/>
       <c r="E232" s="9"/>
     </row>
-    <row r="233">
+    <row r="233" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C233" s="9"/>
       <c r="E233" s="9"/>
     </row>
-    <row r="234">
+    <row r="234" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C234" s="9"/>
       <c r="E234" s="9"/>
     </row>
-    <row r="235">
+    <row r="235" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C235" s="9"/>
       <c r="E235" s="9"/>
     </row>
-    <row r="236">
+    <row r="236" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C236" s="9"/>
       <c r="E236" s="9"/>
     </row>
-    <row r="237">
+    <row r="237" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C237" s="9"/>
       <c r="E237" s="9"/>
     </row>
-    <row r="238">
+    <row r="238" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C238" s="9"/>
       <c r="E238" s="9"/>
     </row>
-    <row r="239">
+    <row r="239" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C239" s="9"/>
       <c r="E239" s="9"/>
     </row>
-    <row r="240">
+    <row r="240" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C240" s="9"/>
       <c r="E240" s="9"/>
     </row>
-    <row r="241">
+    <row r="241" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C241" s="9"/>
       <c r="E241" s="9"/>
     </row>
-    <row r="242">
+    <row r="242" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C242" s="9"/>
       <c r="E242" s="9"/>
     </row>
-    <row r="243">
+    <row r="243" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C243" s="9"/>
       <c r="E243" s="9"/>
     </row>
-    <row r="244">
+    <row r="244" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C244" s="9"/>
       <c r="E244" s="9"/>
     </row>
-    <row r="245">
+    <row r="245" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C245" s="9"/>
       <c r="E245" s="9"/>
     </row>
-    <row r="246">
+    <row r="246" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C246" s="9"/>
       <c r="E246" s="9"/>
     </row>
-    <row r="247">
+    <row r="247" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C247" s="9"/>
       <c r="E247" s="9"/>
     </row>
-    <row r="248">
+    <row r="248" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C248" s="9"/>
       <c r="E248" s="9"/>
     </row>
-    <row r="249">
+    <row r="249" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C249" s="9"/>
       <c r="E249" s="9"/>
     </row>
-    <row r="250">
+    <row r="250" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C250" s="9"/>
       <c r="E250" s="9"/>
     </row>
-    <row r="251">
+    <row r="251" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C251" s="9"/>
       <c r="E251" s="9"/>
     </row>
-    <row r="252">
+    <row r="252" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C252" s="9"/>
       <c r="E252" s="9"/>
     </row>
-    <row r="253">
+    <row r="253" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C253" s="9"/>
       <c r="E253" s="9"/>
     </row>
-    <row r="254">
+    <row r="254" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C254" s="9"/>
       <c r="E254" s="9"/>
     </row>
-    <row r="255">
+    <row r="255" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C255" s="9"/>
       <c r="E255" s="9"/>
     </row>
-    <row r="256">
+    <row r="256" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C256" s="9"/>
       <c r="E256" s="9"/>
     </row>
-    <row r="257">
+    <row r="257" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C257" s="9"/>
       <c r="E257" s="9"/>
     </row>
-    <row r="258">
+    <row r="258" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C258" s="9"/>
       <c r="E258" s="9"/>
     </row>
-    <row r="259">
+    <row r="259" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C259" s="9"/>
       <c r="E259" s="9"/>
     </row>
-    <row r="260">
+    <row r="260" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C260" s="9"/>
       <c r="E260" s="9"/>
     </row>
-    <row r="261">
+    <row r="261" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C261" s="9"/>
       <c r="E261" s="9"/>
     </row>
-    <row r="262">
+    <row r="262" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C262" s="9"/>
       <c r="E262" s="9"/>
     </row>
-    <row r="263">
+    <row r="263" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C263" s="9"/>
       <c r="E263" s="9"/>
     </row>
-    <row r="264">
+    <row r="264" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C264" s="9"/>
       <c r="E264" s="9"/>
     </row>
-    <row r="265">
+    <row r="265" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C265" s="9"/>
       <c r="E265" s="9"/>
     </row>
-    <row r="266">
+    <row r="266" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C266" s="9"/>
       <c r="E266" s="9"/>
     </row>
-    <row r="267">
+    <row r="267" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C267" s="9"/>
       <c r="E267" s="9"/>
     </row>
-    <row r="268">
+    <row r="268" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C268" s="9"/>
       <c r="E268" s="9"/>
     </row>
-    <row r="269">
+    <row r="269" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C269" s="9"/>
       <c r="E269" s="9"/>
     </row>
-    <row r="270">
+    <row r="270" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C270" s="9"/>
       <c r="E270" s="9"/>
     </row>
-    <row r="271">
+    <row r="271" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C271" s="9"/>
       <c r="E271" s="9"/>
     </row>
-    <row r="272">
+    <row r="272" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C272" s="9"/>
       <c r="E272" s="9"/>
     </row>
-    <row r="273">
+    <row r="273" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C273" s="9"/>
       <c r="E273" s="9"/>
     </row>
-    <row r="274">
+    <row r="274" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C274" s="9"/>
       <c r="E274" s="9"/>
     </row>
-    <row r="275">
+    <row r="275" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C275" s="9"/>
       <c r="E275" s="9"/>
     </row>
-    <row r="276">
+    <row r="276" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C276" s="9"/>
       <c r="E276" s="9"/>
     </row>
-    <row r="277">
+    <row r="277" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C277" s="9"/>
       <c r="E277" s="9"/>
     </row>
-    <row r="278">
+    <row r="278" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C278" s="9"/>
       <c r="E278" s="9"/>
     </row>
-    <row r="279">
+    <row r="279" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C279" s="9"/>
       <c r="E279" s="9"/>
     </row>
-    <row r="280">
+    <row r="280" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C280" s="9"/>
       <c r="E280" s="9"/>
     </row>
-    <row r="281">
+    <row r="281" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C281" s="9"/>
       <c r="E281" s="9"/>
     </row>
-    <row r="282">
+    <row r="282" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C282" s="9"/>
       <c r="E282" s="9"/>
     </row>
-    <row r="283">
+    <row r="283" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C283" s="9"/>
       <c r="E283" s="9"/>
     </row>
-    <row r="284">
+    <row r="284" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C284" s="9"/>
       <c r="E284" s="9"/>
     </row>
-    <row r="285">
+    <row r="285" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C285" s="9"/>
       <c r="E285" s="9"/>
     </row>
-    <row r="286">
+    <row r="286" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C286" s="9"/>
       <c r="E286" s="9"/>
     </row>
-    <row r="287">
+    <row r="287" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C287" s="9"/>
       <c r="E287" s="9"/>
     </row>
-    <row r="288">
+    <row r="288" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C288" s="9"/>
       <c r="E288" s="9"/>
     </row>
-    <row r="289">
+    <row r="289" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C289" s="9"/>
       <c r="E289" s="9"/>
     </row>
-    <row r="290">
+    <row r="290" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C290" s="9"/>
       <c r="E290" s="9"/>
     </row>
-    <row r="291">
+    <row r="291" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C291" s="9"/>
       <c r="E291" s="9"/>
     </row>
-    <row r="292">
+    <row r="292" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C292" s="9"/>
       <c r="E292" s="9"/>
     </row>
-    <row r="293">
+    <row r="293" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C293" s="9"/>
       <c r="E293" s="9"/>
     </row>
-    <row r="294">
+    <row r="294" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C294" s="9"/>
       <c r="E294" s="9"/>
     </row>
-    <row r="295">
+    <row r="295" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C295" s="9"/>
       <c r="E295" s="9"/>
     </row>
-    <row r="296">
+    <row r="296" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C296" s="9"/>
       <c r="E296" s="9"/>
     </row>
-    <row r="297">
+    <row r="297" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C297" s="9"/>
       <c r="E297" s="9"/>
     </row>
-    <row r="298">
+    <row r="298" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C298" s="9"/>
       <c r="E298" s="9"/>
     </row>
-    <row r="299">
+    <row r="299" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C299" s="9"/>
       <c r="E299" s="9"/>
     </row>
-    <row r="300">
+    <row r="300" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C300" s="9"/>
       <c r="E300" s="9"/>
     </row>
-    <row r="301">
+    <row r="301" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C301" s="9"/>
       <c r="E301" s="9"/>
     </row>
-    <row r="302">
+    <row r="302" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C302" s="9"/>
       <c r="E302" s="9"/>
     </row>
-    <row r="303">
+    <row r="303" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C303" s="9"/>
       <c r="E303" s="9"/>
     </row>
-    <row r="304">
+    <row r="304" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C304" s="9"/>
       <c r="E304" s="9"/>
     </row>
-    <row r="305">
+    <row r="305" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C305" s="9"/>
       <c r="E305" s="9"/>
     </row>
-    <row r="306">
+    <row r="306" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C306" s="9"/>
       <c r="E306" s="9"/>
     </row>
-    <row r="307">
+    <row r="307" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C307" s="9"/>
       <c r="E307" s="9"/>
     </row>
-    <row r="308">
+    <row r="308" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C308" s="9"/>
       <c r="E308" s="9"/>
     </row>
-    <row r="309">
+    <row r="309" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C309" s="9"/>
       <c r="E309" s="9"/>
     </row>
-    <row r="310">
+    <row r="310" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C310" s="9"/>
       <c r="E310" s="9"/>
     </row>
-    <row r="311">
+    <row r="311" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C311" s="9"/>
       <c r="E311" s="9"/>
     </row>
-    <row r="312">
+    <row r="312" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C312" s="9"/>
       <c r="E312" s="9"/>
     </row>
-    <row r="313">
+    <row r="313" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C313" s="9"/>
       <c r="E313" s="9"/>
     </row>
-    <row r="314">
+    <row r="314" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C314" s="9"/>
       <c r="E314" s="9"/>
     </row>
-    <row r="315">
+    <row r="315" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C315" s="9"/>
       <c r="E315" s="9"/>
     </row>
-    <row r="316">
+    <row r="316" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C316" s="9"/>
       <c r="E316" s="9"/>
     </row>
-    <row r="317">
+    <row r="317" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C317" s="9"/>
       <c r="E317" s="9"/>
     </row>
-    <row r="318">
+    <row r="318" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C318" s="9"/>
       <c r="E318" s="9"/>
     </row>
-    <row r="319">
+    <row r="319" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C319" s="9"/>
       <c r="E319" s="9"/>
     </row>
-    <row r="320">
+    <row r="320" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C320" s="9"/>
       <c r="E320" s="9"/>
     </row>
-    <row r="321">
+    <row r="321" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C321" s="9"/>
       <c r="E321" s="9"/>
     </row>
-    <row r="322">
+    <row r="322" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C322" s="9"/>
       <c r="E322" s="9"/>
     </row>
-    <row r="323">
+    <row r="323" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C323" s="9"/>
       <c r="E323" s="9"/>
     </row>
-    <row r="324">
+    <row r="324" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C324" s="9"/>
       <c r="E324" s="9"/>
     </row>
-    <row r="325">
+    <row r="325" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C325" s="9"/>
       <c r="E325" s="9"/>
     </row>
-    <row r="326">
+    <row r="326" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C326" s="9"/>
       <c r="E326" s="9"/>
     </row>
-    <row r="327">
+    <row r="327" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C327" s="9"/>
       <c r="E327" s="9"/>
     </row>
-    <row r="328">
+    <row r="328" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C328" s="9"/>
       <c r="E328" s="9"/>
     </row>
-    <row r="329">
+    <row r="329" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C329" s="9"/>
       <c r="E329" s="9"/>
     </row>
-    <row r="330">
+    <row r="330" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C330" s="9"/>
       <c r="E330" s="9"/>
     </row>
-    <row r="331">
+    <row r="331" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C331" s="9"/>
       <c r="E331" s="9"/>
     </row>
-    <row r="332">
+    <row r="332" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C332" s="9"/>
       <c r="E332" s="9"/>
     </row>
-    <row r="333">
+    <row r="333" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C333" s="9"/>
       <c r="E333" s="9"/>
     </row>
-    <row r="334">
+    <row r="334" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C334" s="9"/>
       <c r="E334" s="9"/>
     </row>
-    <row r="335">
+    <row r="335" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C335" s="9"/>
       <c r="E335" s="9"/>
     </row>
-    <row r="336">
+    <row r="336" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C336" s="9"/>
       <c r="E336" s="9"/>
     </row>
-    <row r="337">
+    <row r="337" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C337" s="9"/>
       <c r="E337" s="9"/>
     </row>
-    <row r="338">
+    <row r="338" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C338" s="9"/>
       <c r="E338" s="9"/>
     </row>
-    <row r="339">
+    <row r="339" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C339" s="9"/>
       <c r="E339" s="9"/>
     </row>
-    <row r="340">
+    <row r="340" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C340" s="9"/>
       <c r="E340" s="9"/>
     </row>
-    <row r="341">
+    <row r="341" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C341" s="9"/>
       <c r="E341" s="9"/>
     </row>
-    <row r="342">
+    <row r="342" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C342" s="9"/>
       <c r="E342" s="9"/>
     </row>
-    <row r="343">
+    <row r="343" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C343" s="9"/>
       <c r="E343" s="9"/>
     </row>
-    <row r="344">
+    <row r="344" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C344" s="9"/>
       <c r="E344" s="9"/>
     </row>
-    <row r="345">
+    <row r="345" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C345" s="9"/>
       <c r="E345" s="9"/>
     </row>
-    <row r="346">
+    <row r="346" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C346" s="9"/>
       <c r="E346" s="9"/>
     </row>
-    <row r="347">
+    <row r="347" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C347" s="9"/>
       <c r="E347" s="9"/>
     </row>
-    <row r="348">
+    <row r="348" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C348" s="9"/>
       <c r="E348" s="9"/>
     </row>
-    <row r="349">
+    <row r="349" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C349" s="9"/>
       <c r="E349" s="9"/>
     </row>
-    <row r="350">
+    <row r="350" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C350" s="9"/>
       <c r="E350" s="9"/>
     </row>
-    <row r="351">
+    <row r="351" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C351" s="9"/>
       <c r="E351" s="9"/>
     </row>
-    <row r="352">
+    <row r="352" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C352" s="9"/>
       <c r="E352" s="9"/>
     </row>
-    <row r="353">
+    <row r="353" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C353" s="9"/>
       <c r="E353" s="9"/>
     </row>
-    <row r="354">
+    <row r="354" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C354" s="9"/>
       <c r="E354" s="9"/>
     </row>
-    <row r="355">
+    <row r="355" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C355" s="9"/>
       <c r="E355" s="9"/>
     </row>
-    <row r="356">
+    <row r="356" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C356" s="9"/>
       <c r="E356" s="9"/>
     </row>
-    <row r="357">
+    <row r="357" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C357" s="9"/>
       <c r="E357" s="9"/>
     </row>
-    <row r="358">
+    <row r="358" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C358" s="9"/>
       <c r="E358" s="9"/>
     </row>
-    <row r="359">
+    <row r="359" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C359" s="9"/>
       <c r="E359" s="9"/>
     </row>
-    <row r="360">
+    <row r="360" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C360" s="9"/>
       <c r="E360" s="9"/>
     </row>
-    <row r="361">
+    <row r="361" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C361" s="9"/>
       <c r="E361" s="9"/>
     </row>
-    <row r="362">
+    <row r="362" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C362" s="9"/>
       <c r="E362" s="9"/>
     </row>
-    <row r="363">
+    <row r="363" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C363" s="9"/>
       <c r="E363" s="9"/>
     </row>
-    <row r="364">
+    <row r="364" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C364" s="9"/>
       <c r="E364" s="9"/>
     </row>
-    <row r="365">
+    <row r="365" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C365" s="9"/>
       <c r="E365" s="9"/>
     </row>
-    <row r="366">
+    <row r="366" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C366" s="9"/>
       <c r="E366" s="9"/>
     </row>
-    <row r="367">
+    <row r="367" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C367" s="9"/>
       <c r="E367" s="9"/>
     </row>
-    <row r="368">
+    <row r="368" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C368" s="9"/>
       <c r="E368" s="9"/>
     </row>
-    <row r="369">
+    <row r="369" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C369" s="9"/>
       <c r="E369" s="9"/>
     </row>
-    <row r="370">
+    <row r="370" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C370" s="9"/>
       <c r="E370" s="9"/>
     </row>
-    <row r="371">
+    <row r="371" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C371" s="9"/>
       <c r="E371" s="9"/>
     </row>
-    <row r="372">
+    <row r="372" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C372" s="9"/>
       <c r="E372" s="9"/>
     </row>
-    <row r="373">
+    <row r="373" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C373" s="9"/>
       <c r="E373" s="9"/>
     </row>
-    <row r="374">
+    <row r="374" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C374" s="9"/>
       <c r="E374" s="9"/>
     </row>
-    <row r="375">
+    <row r="375" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C375" s="9"/>
       <c r="E375" s="9"/>
     </row>
-    <row r="376">
+    <row r="376" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C376" s="9"/>
       <c r="E376" s="9"/>
     </row>
-    <row r="377">
+    <row r="377" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C377" s="9"/>
       <c r="E377" s="9"/>
     </row>
-    <row r="378">
+    <row r="378" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C378" s="9"/>
       <c r="E378" s="9"/>
     </row>
-    <row r="379">
+    <row r="379" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C379" s="9"/>
       <c r="E379" s="9"/>
     </row>
-    <row r="380">
+    <row r="380" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C380" s="9"/>
       <c r="E380" s="9"/>
     </row>
-    <row r="381">
+    <row r="381" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C381" s="9"/>
       <c r="E381" s="9"/>
     </row>
-    <row r="382">
+    <row r="382" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C382" s="9"/>
       <c r="E382" s="9"/>
     </row>
-    <row r="383">
+    <row r="383" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C383" s="9"/>
       <c r="E383" s="9"/>
     </row>
-    <row r="384">
+    <row r="384" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C384" s="9"/>
       <c r="E384" s="9"/>
     </row>
-    <row r="385">
+    <row r="385" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C385" s="9"/>
       <c r="E385" s="9"/>
     </row>
-    <row r="386">
+    <row r="386" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C386" s="9"/>
       <c r="E386" s="9"/>
     </row>
-    <row r="387">
+    <row r="387" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C387" s="9"/>
       <c r="E387" s="9"/>
     </row>
-    <row r="388">
+    <row r="388" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C388" s="9"/>
       <c r="E388" s="9"/>
     </row>
-    <row r="389">
+    <row r="389" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C389" s="9"/>
       <c r="E389" s="9"/>
     </row>
-    <row r="390">
+    <row r="390" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C390" s="9"/>
       <c r="E390" s="9"/>
     </row>
-    <row r="391">
+    <row r="391" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C391" s="9"/>
       <c r="E391" s="9"/>
     </row>
-    <row r="392">
+    <row r="392" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C392" s="9"/>
       <c r="E392" s="9"/>
     </row>
-    <row r="393">
+    <row r="393" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C393" s="9"/>
       <c r="E393" s="9"/>
     </row>
-    <row r="394">
+    <row r="394" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C394" s="9"/>
       <c r="E394" s="9"/>
     </row>
-    <row r="395">
+    <row r="395" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C395" s="9"/>
       <c r="E395" s="9"/>
     </row>
-    <row r="396">
+    <row r="396" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C396" s="9"/>
       <c r="E396" s="9"/>
     </row>
-    <row r="397">
+    <row r="397" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C397" s="9"/>
       <c r="E397" s="9"/>
     </row>
-    <row r="398">
+    <row r="398" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C398" s="9"/>
       <c r="E398" s="9"/>
     </row>
-    <row r="399">
+    <row r="399" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C399" s="9"/>
       <c r="E399" s="9"/>
     </row>
-    <row r="400">
+    <row r="400" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C400" s="9"/>
       <c r="E400" s="9"/>
     </row>
-    <row r="401">
+    <row r="401" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C401" s="9"/>
       <c r="E401" s="9"/>
     </row>
-    <row r="402">
+    <row r="402" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C402" s="9"/>
       <c r="E402" s="9"/>
     </row>
-    <row r="403">
+    <row r="403" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C403" s="9"/>
       <c r="E403" s="9"/>
     </row>
-    <row r="404">
+    <row r="404" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C404" s="9"/>
       <c r="E404" s="9"/>
     </row>
-    <row r="405">
+    <row r="405" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C405" s="9"/>
       <c r="E405" s="9"/>
     </row>
-    <row r="406">
+    <row r="406" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C406" s="9"/>
       <c r="E406" s="9"/>
     </row>
-    <row r="407">
+    <row r="407" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C407" s="9"/>
       <c r="E407" s="9"/>
     </row>
-    <row r="408">
+    <row r="408" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C408" s="9"/>
       <c r="E408" s="9"/>
     </row>
-    <row r="409">
+    <row r="409" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C409" s="9"/>
       <c r="E409" s="9"/>
     </row>
-    <row r="410">
+    <row r="410" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C410" s="9"/>
       <c r="E410" s="9"/>
     </row>
-    <row r="411">
+    <row r="411" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C411" s="9"/>
       <c r="E411" s="9"/>
     </row>
-    <row r="412">
+    <row r="412" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C412" s="9"/>
       <c r="E412" s="9"/>
     </row>
-    <row r="413">
+    <row r="413" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C413" s="9"/>
       <c r="E413" s="9"/>
     </row>
-    <row r="414">
+    <row r="414" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C414" s="9"/>
       <c r="E414" s="9"/>
     </row>
-    <row r="415">
+    <row r="415" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C415" s="9"/>
       <c r="E415" s="9"/>
     </row>
-    <row r="416">
+    <row r="416" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C416" s="9"/>
       <c r="E416" s="9"/>
     </row>
-    <row r="417">
+    <row r="417" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C417" s="9"/>
       <c r="E417" s="9"/>
     </row>
-    <row r="418">
+    <row r="418" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C418" s="9"/>
       <c r="E418" s="9"/>
     </row>
-    <row r="419">
+    <row r="419" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C419" s="9"/>
       <c r="E419" s="9"/>
     </row>
-    <row r="420">
+    <row r="420" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C420" s="9"/>
       <c r="E420" s="9"/>
     </row>
-    <row r="421">
+    <row r="421" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C421" s="9"/>
       <c r="E421" s="9"/>
     </row>
-    <row r="422">
+    <row r="422" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C422" s="9"/>
       <c r="E422" s="9"/>
     </row>
-    <row r="423">
+    <row r="423" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C423" s="9"/>
       <c r="E423" s="9"/>
     </row>
-    <row r="424">
+    <row r="424" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C424" s="9"/>
       <c r="E424" s="9"/>
     </row>
-    <row r="425">
+    <row r="425" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C425" s="9"/>
       <c r="E425" s="9"/>
     </row>
-    <row r="426">
+    <row r="426" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C426" s="9"/>
       <c r="E426" s="9"/>
     </row>
-    <row r="427">
+    <row r="427" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C427" s="9"/>
       <c r="E427" s="9"/>
     </row>
-    <row r="428">
+    <row r="428" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C428" s="9"/>
       <c r="E428" s="9"/>
     </row>
-    <row r="429">
+    <row r="429" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C429" s="9"/>
       <c r="E429" s="9"/>
     </row>
-    <row r="430">
+    <row r="430" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C430" s="9"/>
       <c r="E430" s="9"/>
     </row>
-    <row r="431">
+    <row r="431" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C431" s="9"/>
       <c r="E431" s="9"/>
     </row>
-    <row r="432">
+    <row r="432" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C432" s="9"/>
       <c r="E432" s="9"/>
     </row>
-    <row r="433">
+    <row r="433" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C433" s="9"/>
       <c r="E433" s="9"/>
     </row>
-    <row r="434">
+    <row r="434" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C434" s="9"/>
       <c r="E434" s="9"/>
     </row>
-    <row r="435">
+    <row r="435" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C435" s="9"/>
       <c r="E435" s="9"/>
     </row>
-    <row r="436">
+    <row r="436" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C436" s="9"/>
       <c r="E436" s="9"/>
     </row>
-    <row r="437">
+    <row r="437" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C437" s="9"/>
       <c r="E437" s="9"/>
     </row>
-    <row r="438">
+    <row r="438" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C438" s="9"/>
       <c r="E438" s="9"/>
     </row>
-    <row r="439">
+    <row r="439" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C439" s="9"/>
       <c r="E439" s="9"/>
     </row>
-    <row r="440">
+    <row r="440" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C440" s="9"/>
       <c r="E440" s="9"/>
     </row>
-    <row r="441">
+    <row r="441" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C441" s="9"/>
       <c r="E441" s="9"/>
     </row>
-    <row r="442">
+    <row r="442" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C442" s="9"/>
       <c r="E442" s="9"/>
     </row>
-    <row r="443">
+    <row r="443" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C443" s="9"/>
       <c r="E443" s="9"/>
     </row>
-    <row r="444">
+    <row r="444" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C444" s="9"/>
       <c r="E444" s="9"/>
     </row>
-    <row r="445">
+    <row r="445" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C445" s="9"/>
       <c r="E445" s="9"/>
     </row>
-    <row r="446">
+    <row r="446" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C446" s="9"/>
       <c r="E446" s="9"/>
     </row>
-    <row r="447">
+    <row r="447" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C447" s="9"/>
       <c r="E447" s="9"/>
     </row>
-    <row r="448">
+    <row r="448" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C448" s="9"/>
       <c r="E448" s="9"/>
     </row>
-    <row r="449">
+    <row r="449" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C449" s="9"/>
       <c r="E449" s="9"/>
     </row>
-    <row r="450">
+    <row r="450" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C450" s="9"/>
       <c r="E450" s="9"/>
     </row>
-    <row r="451">
+    <row r="451" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C451" s="9"/>
       <c r="E451" s="9"/>
     </row>
-    <row r="452">
+    <row r="452" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C452" s="9"/>
       <c r="E452" s="9"/>
     </row>
-    <row r="453">
+    <row r="453" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C453" s="9"/>
       <c r="E453" s="9"/>
     </row>
-    <row r="454">
+    <row r="454" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C454" s="9"/>
       <c r="E454" s="9"/>
     </row>
-    <row r="455">
+    <row r="455" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C455" s="9"/>
       <c r="E455" s="9"/>
     </row>
-    <row r="456">
+    <row r="456" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C456" s="9"/>
       <c r="E456" s="9"/>
     </row>
-    <row r="457">
+    <row r="457" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C457" s="9"/>
       <c r="E457" s="9"/>
     </row>
-    <row r="458">
+    <row r="458" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C458" s="9"/>
       <c r="E458" s="9"/>
     </row>
-    <row r="459">
+    <row r="459" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C459" s="9"/>
       <c r="E459" s="9"/>
     </row>
-    <row r="460">
+    <row r="460" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C460" s="9"/>
       <c r="E460" s="9"/>
     </row>
-    <row r="461">
+    <row r="461" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C461" s="9"/>
       <c r="E461" s="9"/>
     </row>
-    <row r="462">
+    <row r="462" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C462" s="9"/>
       <c r="E462" s="9"/>
     </row>
-    <row r="463">
+    <row r="463" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C463" s="9"/>
       <c r="E463" s="9"/>
     </row>
-    <row r="464">
+    <row r="464" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C464" s="9"/>
       <c r="E464" s="9"/>
     </row>
-    <row r="465">
+    <row r="465" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C465" s="9"/>
       <c r="E465" s="9"/>
     </row>
-    <row r="466">
+    <row r="466" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C466" s="9"/>
       <c r="E466" s="9"/>
     </row>
-    <row r="467">
+    <row r="467" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C467" s="9"/>
       <c r="E467" s="9"/>
     </row>
-    <row r="468">
+    <row r="468" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C468" s="9"/>
       <c r="E468" s="9"/>
     </row>
-    <row r="469">
+    <row r="469" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C469" s="9"/>
       <c r="E469" s="9"/>
     </row>
-    <row r="470">
+    <row r="470" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C470" s="9"/>
       <c r="E470" s="9"/>
     </row>
-    <row r="471">
+    <row r="471" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C471" s="9"/>
       <c r="E471" s="9"/>
     </row>
-    <row r="472">
+    <row r="472" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C472" s="9"/>
       <c r="E472" s="9"/>
     </row>
-    <row r="473">
+    <row r="473" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C473" s="9"/>
       <c r="E473" s="9"/>
     </row>
-    <row r="474">
+    <row r="474" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C474" s="9"/>
       <c r="E474" s="9"/>
     </row>
-    <row r="475">
+    <row r="475" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C475" s="9"/>
       <c r="E475" s="9"/>
     </row>
-    <row r="476">
+    <row r="476" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C476" s="9"/>
       <c r="E476" s="9"/>
     </row>
-    <row r="477">
+    <row r="477" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C477" s="9"/>
       <c r="E477" s="9"/>
     </row>
-    <row r="478">
+    <row r="478" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C478" s="9"/>
       <c r="E478" s="9"/>
     </row>
-    <row r="479">
+    <row r="479" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C479" s="9"/>
       <c r="E479" s="9"/>
     </row>
-    <row r="480">
+    <row r="480" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C480" s="9"/>
       <c r="E480" s="9"/>
     </row>
-    <row r="481">
+    <row r="481" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C481" s="9"/>
       <c r="E481" s="9"/>
     </row>
-    <row r="482">
+    <row r="482" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C482" s="9"/>
       <c r="E482" s="9"/>
     </row>
-    <row r="483">
+    <row r="483" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C483" s="9"/>
       <c r="E483" s="9"/>
     </row>
-    <row r="484">
+    <row r="484" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C484" s="9"/>
       <c r="E484" s="9"/>
     </row>
-    <row r="485">
+    <row r="485" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C485" s="9"/>
       <c r="E485" s="9"/>
     </row>
-    <row r="486">
+    <row r="486" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C486" s="9"/>
       <c r="E486" s="9"/>
     </row>
-    <row r="487">
+    <row r="487" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C487" s="9"/>
       <c r="E487" s="9"/>
     </row>
-    <row r="488">
+    <row r="488" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C488" s="9"/>
       <c r="E488" s="9"/>
     </row>
-    <row r="489">
+    <row r="489" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C489" s="9"/>
       <c r="E489" s="9"/>
     </row>
-    <row r="490">
+    <row r="490" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C490" s="9"/>
       <c r="E490" s="9"/>
     </row>
-    <row r="491">
+    <row r="491" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C491" s="9"/>
       <c r="E491" s="9"/>
     </row>
-    <row r="492">
+    <row r="492" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C492" s="9"/>
       <c r="E492" s="9"/>
     </row>
-    <row r="493">
+    <row r="493" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C493" s="9"/>
       <c r="E493" s="9"/>
     </row>
-    <row r="494">
+    <row r="494" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C494" s="9"/>
       <c r="E494" s="9"/>
     </row>
-    <row r="495">
+    <row r="495" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C495" s="9"/>
       <c r="E495" s="9"/>
     </row>
-    <row r="496">
+    <row r="496" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C496" s="9"/>
       <c r="E496" s="9"/>
     </row>
-    <row r="497">
+    <row r="497" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C497" s="9"/>
       <c r="E497" s="9"/>
     </row>
-    <row r="498">
+    <row r="498" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C498" s="9"/>
       <c r="E498" s="9"/>
     </row>
-    <row r="499">
+    <row r="499" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C499" s="9"/>
       <c r="E499" s="9"/>
     </row>
-    <row r="500">
+    <row r="500" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C500" s="9"/>
       <c r="E500" s="9"/>
     </row>
-    <row r="501">
+    <row r="501" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C501" s="9"/>
       <c r="E501" s="9"/>
     </row>
-    <row r="502">
+    <row r="502" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C502" s="9"/>
       <c r="E502" s="9"/>
     </row>
-    <row r="503">
+    <row r="503" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C503" s="9"/>
       <c r="E503" s="9"/>
     </row>
-    <row r="504">
+    <row r="504" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C504" s="9"/>
       <c r="E504" s="9"/>
     </row>
-    <row r="505">
+    <row r="505" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C505" s="9"/>
       <c r="E505" s="9"/>
     </row>
-    <row r="506">
+    <row r="506" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C506" s="9"/>
       <c r="E506" s="9"/>
     </row>
-    <row r="507">
+    <row r="507" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C507" s="9"/>
       <c r="E507" s="9"/>
     </row>
-    <row r="508">
+    <row r="508" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C508" s="9"/>
       <c r="E508" s="9"/>
     </row>
-    <row r="509">
+    <row r="509" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C509" s="9"/>
       <c r="E509" s="9"/>
     </row>
-    <row r="510">
+    <row r="510" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C510" s="9"/>
       <c r="E510" s="9"/>
     </row>
-    <row r="511">
+    <row r="511" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C511" s="9"/>
       <c r="E511" s="9"/>
     </row>
-    <row r="512">
+    <row r="512" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C512" s="9"/>
       <c r="E512" s="9"/>
     </row>
-    <row r="513">
+    <row r="513" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C513" s="9"/>
       <c r="E513" s="9"/>
     </row>
-    <row r="514">
+    <row r="514" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C514" s="9"/>
       <c r="E514" s="9"/>
     </row>
-    <row r="515">
+    <row r="515" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C515" s="9"/>
       <c r="E515" s="9"/>
     </row>
-    <row r="516">
+    <row r="516" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C516" s="9"/>
       <c r="E516" s="9"/>
     </row>
-    <row r="517">
+    <row r="517" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C517" s="9"/>
       <c r="E517" s="9"/>
     </row>
-    <row r="518">
+    <row r="518" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C518" s="9"/>
       <c r="E518" s="9"/>
     </row>
-    <row r="519">
+    <row r="519" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C519" s="9"/>
       <c r="E519" s="9"/>
     </row>
-    <row r="520">
+    <row r="520" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C520" s="9"/>
       <c r="E520" s="9"/>
     </row>
-    <row r="521">
+    <row r="521" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C521" s="9"/>
       <c r="E521" s="9"/>
     </row>
-    <row r="522">
+    <row r="522" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C522" s="9"/>
       <c r="E522" s="9"/>
     </row>
-    <row r="523">
+    <row r="523" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C523" s="9"/>
       <c r="E523" s="9"/>
     </row>
-    <row r="524">
+    <row r="524" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C524" s="9"/>
       <c r="E524" s="9"/>
     </row>
-    <row r="525">
+    <row r="525" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C525" s="9"/>
       <c r="E525" s="9"/>
     </row>
-    <row r="526">
+    <row r="526" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C526" s="9"/>
       <c r="E526" s="9"/>
     </row>
-    <row r="527">
+    <row r="527" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C527" s="9"/>
       <c r="E527" s="9"/>
     </row>
-    <row r="528">
+    <row r="528" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C528" s="9"/>
       <c r="E528" s="9"/>
     </row>
-    <row r="529">
+    <row r="529" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C529" s="9"/>
       <c r="E529" s="9"/>
     </row>
-    <row r="530">
+    <row r="530" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C530" s="9"/>
       <c r="E530" s="9"/>
     </row>
-    <row r="531">
+    <row r="531" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C531" s="9"/>
       <c r="E531" s="9"/>
     </row>
-    <row r="532">
+    <row r="532" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C532" s="9"/>
       <c r="E532" s="9"/>
     </row>
-    <row r="533">
+    <row r="533" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C533" s="9"/>
       <c r="E533" s="9"/>
     </row>
-    <row r="534">
+    <row r="534" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C534" s="9"/>
       <c r="E534" s="9"/>
     </row>
-    <row r="535">
+    <row r="535" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C535" s="9"/>
       <c r="E535" s="9"/>
     </row>
-    <row r="536">
+    <row r="536" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C536" s="9"/>
       <c r="E536" s="9"/>
     </row>
-    <row r="537">
+    <row r="537" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C537" s="9"/>
       <c r="E537" s="9"/>
     </row>
-    <row r="538">
+    <row r="538" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C538" s="9"/>
       <c r="E538" s="9"/>
     </row>
-    <row r="539">
+    <row r="539" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C539" s="9"/>
       <c r="E539" s="9"/>
     </row>
-    <row r="540">
+    <row r="540" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C540" s="9"/>
       <c r="E540" s="9"/>
     </row>
-    <row r="541">
+    <row r="541" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C541" s="9"/>
       <c r="E541" s="9"/>
     </row>
-    <row r="542">
+    <row r="542" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C542" s="9"/>
       <c r="E542" s="9"/>
     </row>
-    <row r="543">
+    <row r="543" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C543" s="9"/>
       <c r="E543" s="9"/>
     </row>
-    <row r="544">
+    <row r="544" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C544" s="9"/>
       <c r="E544" s="9"/>
     </row>
-    <row r="545">
+    <row r="545" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C545" s="9"/>
       <c r="E545" s="9"/>
     </row>
-    <row r="546">
+    <row r="546" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C546" s="9"/>
       <c r="E546" s="9"/>
     </row>
-    <row r="547">
+    <row r="547" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C547" s="9"/>
       <c r="E547" s="9"/>
     </row>
-    <row r="548">
+    <row r="548" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C548" s="9"/>
       <c r="E548" s="9"/>
     </row>
-    <row r="549">
+    <row r="549" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C549" s="9"/>
       <c r="E549" s="9"/>
     </row>
-    <row r="550">
+    <row r="550" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C550" s="9"/>
       <c r="E550" s="9"/>
     </row>
-    <row r="551">
+    <row r="551" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C551" s="9"/>
       <c r="E551" s="9"/>
     </row>
-    <row r="552">
+    <row r="552" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C552" s="9"/>
       <c r="E552" s="9"/>
     </row>
-    <row r="553">
+    <row r="553" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C553" s="9"/>
       <c r="E553" s="9"/>
     </row>
-    <row r="554">
+    <row r="554" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C554" s="9"/>
       <c r="E554" s="9"/>
     </row>
-    <row r="555">
+    <row r="555" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C555" s="9"/>
       <c r="E555" s="9"/>
     </row>
-    <row r="556">
+    <row r="556" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C556" s="9"/>
       <c r="E556" s="9"/>
     </row>
-    <row r="557">
+    <row r="557" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C557" s="9"/>
       <c r="E557" s="9"/>
     </row>
-    <row r="558">
+    <row r="558" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C558" s="9"/>
       <c r="E558" s="9"/>
     </row>
-    <row r="559">
+    <row r="559" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C559" s="9"/>
       <c r="E559" s="9"/>
     </row>
-    <row r="560">
+    <row r="560" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C560" s="9"/>
       <c r="E560" s="9"/>
     </row>
-    <row r="561">
+    <row r="561" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C561" s="9"/>
       <c r="E561" s="9"/>
     </row>
-    <row r="562">
+    <row r="562" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C562" s="9"/>
       <c r="E562" s="9"/>
     </row>
-    <row r="563">
+    <row r="563" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C563" s="9"/>
       <c r="E563" s="9"/>
     </row>
-    <row r="564">
+    <row r="564" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C564" s="9"/>
       <c r="E564" s="9"/>
     </row>
-    <row r="565">
+    <row r="565" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C565" s="9"/>
       <c r="E565" s="9"/>
     </row>
-    <row r="566">
+    <row r="566" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C566" s="9"/>
       <c r="E566" s="9"/>
     </row>
-    <row r="567">
+    <row r="567" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C567" s="9"/>
       <c r="E567" s="9"/>
     </row>
-    <row r="568">
+    <row r="568" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C568" s="9"/>
       <c r="E568" s="9"/>
     </row>
-    <row r="569">
+    <row r="569" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C569" s="9"/>
       <c r="E569" s="9"/>
     </row>
-    <row r="570">
+    <row r="570" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C570" s="9"/>
       <c r="E570" s="9"/>
     </row>
-    <row r="571">
+    <row r="571" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C571" s="9"/>
       <c r="E571" s="9"/>
     </row>
-    <row r="572">
+    <row r="572" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C572" s="9"/>
       <c r="E572" s="9"/>
     </row>
-    <row r="573">
+    <row r="573" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C573" s="9"/>
       <c r="E573" s="9"/>
     </row>
-    <row r="574">
+    <row r="574" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C574" s="9"/>
       <c r="E574" s="9"/>
     </row>
-    <row r="575">
+    <row r="575" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C575" s="9"/>
       <c r="E575" s="9"/>
     </row>
-    <row r="576">
+    <row r="576" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C576" s="9"/>
       <c r="E576" s="9"/>
     </row>
-    <row r="577">
+    <row r="577" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C577" s="9"/>
       <c r="E577" s="9"/>
     </row>
-    <row r="578">
+    <row r="578" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C578" s="9"/>
       <c r="E578" s="9"/>
     </row>
-    <row r="579">
+    <row r="579" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C579" s="9"/>
       <c r="E579" s="9"/>
     </row>
-    <row r="580">
+    <row r="580" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C580" s="9"/>
       <c r="E580" s="9"/>
     </row>
-    <row r="581">
+    <row r="581" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C581" s="9"/>
       <c r="E581" s="9"/>
     </row>
-    <row r="582">
+    <row r="582" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C582" s="9"/>
       <c r="E582" s="9"/>
     </row>
-    <row r="583">
+    <row r="583" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C583" s="9"/>
       <c r="E583" s="9"/>
     </row>
-    <row r="584">
+    <row r="584" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C584" s="9"/>
       <c r="E584" s="9"/>
     </row>
-    <row r="585">
+    <row r="585" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C585" s="9"/>
       <c r="E585" s="9"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D9:D585 F9:F585">
-    <cfRule priority="1" stopIfTrue="1" dxfId="0" type="expression">
-      <formula>AND(ISBLANK(D9),C9="Pass")</formula>
+  <conditionalFormatting sqref="C2:C585 E2:E585">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>"Pass"</formula>
     </cfRule>
-    <cfRule priority="3" stopIfTrue="1" dxfId="1" type="expression">
-      <formula>AND(ISBLANK(D9),C9="Fail")</formula>
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+      <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D8 F2:F8">
-    <cfRule priority="2" stopIfTrue="1" dxfId="0" type="expression">
+  <conditionalFormatting sqref="D2:D585 F2:F585">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
-    <cfRule priority="4" stopIfTrue="1" dxfId="1" type="expression">
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C585 E2:E585">
-    <cfRule priority="5" dxfId="2" type="cellIs" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule priority="6" dxfId="3" type="cellIs" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C585 E2:E585">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C585 E2:E585" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup r:id="rId1" orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sprint 3 Acceptence Test Plan inital update.
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\team-project-2245-swen-261-04-6f\etc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\water\Favorites\team-project-2245-swen-261-04-6f\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4D67DC-940F-47FB-809B-6462C350850E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B584A442-6F91-4168-B75C-129066A3206C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
   <si>
     <t>Instructions</t>
   </si>
@@ -537,6 +537,39 @@
   </si>
   <si>
     <t>not implemented yet</t>
+  </si>
+  <si>
+    <t>As a Helper, I want to see a list of all available needs so that I can decide which ones to support.</t>
+  </si>
+  <si>
+    <t>Given I am logged in as a Helper, when I visit the needs page, then I will see a list of all available needs.</t>
+  </si>
+  <si>
+    <t>Given there are no needs available, when I visit the needs page, then I will see a message stating no needs are currently listed.</t>
+  </si>
+  <si>
+    <t>As a Helper, I want to check out and fund my selected needs so that I can complete my contribution.</t>
+  </si>
+  <si>
+    <t>As a USER I want to SAVE CHANGES so that I DONT HAVE TO RESTART every time I start the program again.</t>
+  </si>
+  <si>
+    <t>Given a helper adds items to their basket, when they logout and log back in and/or the program ends and starts again, then their funding basket should be saved.</t>
+  </si>
+  <si>
+    <t>Given an admin adds a need to the cupboard, when the program ends and starts again, then the needs in the cupboard should be saved.</t>
+  </si>
+  <si>
+    <t>Given I confirm the checkout, when I complete the process, then my basket is cleared, and the needs are marked as funded.</t>
+  </si>
+  <si>
+    <t>Given I log out and log back in, when I visit my basket, then I see an empty basket after a successful checkout.</t>
+  </si>
+  <si>
+    <t>E.L.; 04/07/2025;</t>
+  </si>
+  <si>
+    <t>E.Z.W.; 04/07/2025;</t>
   </si>
 </sst>
 </file>
@@ -1004,13 +1037,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21" style="2" customWidth="1"/>
-    <col min="2" max="2" width="106.83203125" customWidth="1"/>
+    <col min="2" max="2" width="106.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="279" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="280.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1018,7 +1051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1026,7 +1059,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1044,12 +1077,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F585"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A21" sqref="A21"/>
+      <selection pane="topRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" style="4" customWidth="1"/>
     <col min="2" max="2" width="60" style="4" customWidth="1"/>
@@ -1057,10 +1090,10 @@
     <col min="4" max="4" width="60" style="4" customWidth="1"/>
     <col min="5" max="5" width="9" style="4" customWidth="1"/>
     <col min="6" max="6" width="60" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="6"/>
+    <col min="7" max="16384" width="10.796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -1080,7 +1113,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="46.2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
@@ -1095,7 +1128,7 @@
       </c>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
@@ -1108,7 +1141,7 @@
       </c>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="4" t="s">
         <v>16</v>
@@ -1121,7 +1154,7 @@
       </c>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="4" t="s">
         <v>18</v>
@@ -1134,7 +1167,7 @@
       </c>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="4" t="s">
         <v>19</v>
@@ -1147,7 +1180,7 @@
       </c>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="62" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>20</v>
       </c>
@@ -1162,7 +1195,7 @@
       </c>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>23</v>
       </c>
@@ -1174,7 +1207,7 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:6" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
@@ -1189,7 +1222,7 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1201,7 +1234,7 @@
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
@@ -1213,7 +1246,7 @@
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
@@ -1225,7 +1258,7 @@
       </c>
       <c r="E12" s="9"/>
     </row>
-    <row r="13" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>30</v>
       </c>
@@ -1237,7 +1270,7 @@
       </c>
       <c r="E13" s="9"/>
     </row>
-    <row r="14" spans="1:6" ht="62" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -1252,7 +1285,7 @@
       </c>
       <c r="E14" s="9"/>
     </row>
-    <row r="15" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>34</v>
       </c>
@@ -1264,7 +1297,7 @@
       </c>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>35</v>
       </c>
@@ -1277,2300 +1310,2361 @@
       </c>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="D17" s="4" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E17" s="9"/>
     </row>
-    <row r="18" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="9"/>
+      <c r="C18" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="D18" s="4" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="D19" s="4" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C20" s="9"/>
+    <row r="20" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="E20" s="9"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B21" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="C21" s="9"/>
       <c r="E21" s="9"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="C22" s="9"/>
       <c r="E22" s="9"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C23" s="9"/>
+    <row r="23" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="E23" s="9"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C24" s="9"/>
+    <row r="24" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="E24" s="9"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C25" s="9"/>
+    <row r="25" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C26" s="9"/>
+    <row r="26" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="E26" s="9"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C27" s="9"/>
       <c r="E27" s="9"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C28" s="9"/>
       <c r="E28" s="9"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C29" s="9"/>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C30" s="9"/>
       <c r="E30" s="9"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C31" s="9"/>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C32" s="9"/>
       <c r="E32" s="9"/>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C33" s="9"/>
       <c r="E33" s="9"/>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C34" s="9"/>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C35" s="9"/>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C36" s="9"/>
       <c r="E36" s="9"/>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C37" s="9"/>
       <c r="E37" s="9"/>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C38" s="9"/>
       <c r="E38" s="9"/>
     </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C39" s="9"/>
       <c r="E39" s="9"/>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C40" s="9"/>
       <c r="E40" s="9"/>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C41" s="9"/>
       <c r="E41" s="9"/>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C42" s="9"/>
       <c r="E42" s="9"/>
     </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C43" s="9"/>
       <c r="E43" s="9"/>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C44" s="9"/>
       <c r="E44" s="9"/>
     </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C45" s="9"/>
       <c r="E45" s="9"/>
     </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C46" s="9"/>
       <c r="E46" s="9"/>
     </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C47" s="9"/>
       <c r="E47" s="9"/>
     </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C48" s="9"/>
       <c r="E48" s="9"/>
     </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C49" s="9"/>
       <c r="E49" s="9"/>
     </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C50" s="9"/>
       <c r="E50" s="9"/>
     </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C51" s="9"/>
       <c r="E51" s="9"/>
     </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C52" s="9"/>
       <c r="E52" s="9"/>
     </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C53" s="9"/>
       <c r="E53" s="9"/>
     </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C54" s="9"/>
       <c r="E54" s="9"/>
     </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C55" s="9"/>
       <c r="E55" s="9"/>
     </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C56" s="9"/>
       <c r="E56" s="9"/>
     </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C57" s="9"/>
       <c r="E57" s="9"/>
     </row>
-    <row r="58" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C58" s="9"/>
       <c r="E58" s="9"/>
     </row>
-    <row r="59" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C59" s="9"/>
       <c r="E59" s="9"/>
     </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C60" s="9"/>
       <c r="E60" s="9"/>
     </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C61" s="9"/>
       <c r="E61" s="9"/>
     </row>
-    <row r="62" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C62" s="9"/>
       <c r="E62" s="9"/>
     </row>
-    <row r="63" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C63" s="9"/>
       <c r="E63" s="9"/>
     </row>
-    <row r="64" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C64" s="9"/>
       <c r="E64" s="9"/>
     </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C65" s="9"/>
       <c r="E65" s="9"/>
     </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C66" s="9"/>
       <c r="E66" s="9"/>
     </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C67" s="9"/>
       <c r="E67" s="9"/>
     </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C68" s="9"/>
       <c r="E68" s="9"/>
     </row>
-    <row r="69" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C69" s="9"/>
       <c r="E69" s="9"/>
     </row>
-    <row r="70" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C70" s="9"/>
       <c r="E70" s="9"/>
     </row>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C71" s="9"/>
       <c r="E71" s="9"/>
     </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C72" s="9"/>
       <c r="E72" s="9"/>
     </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C73" s="9"/>
       <c r="E73" s="9"/>
     </row>
-    <row r="74" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C74" s="9"/>
       <c r="E74" s="9"/>
     </row>
-    <row r="75" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C75" s="9"/>
       <c r="E75" s="9"/>
     </row>
-    <row r="76" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C76" s="9"/>
       <c r="E76" s="9"/>
     </row>
-    <row r="77" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C77" s="9"/>
       <c r="E77" s="9"/>
     </row>
-    <row r="78" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C78" s="9"/>
       <c r="E78" s="9"/>
     </row>
-    <row r="79" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C79" s="9"/>
       <c r="E79" s="9"/>
     </row>
-    <row r="80" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C80" s="9"/>
       <c r="E80" s="9"/>
     </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C81" s="9"/>
       <c r="E81" s="9"/>
     </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C82" s="9"/>
       <c r="E82" s="9"/>
     </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C83" s="9"/>
       <c r="E83" s="9"/>
     </row>
-    <row r="84" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C84" s="9"/>
       <c r="E84" s="9"/>
     </row>
-    <row r="85" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C85" s="9"/>
       <c r="E85" s="9"/>
     </row>
-    <row r="86" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C86" s="9"/>
       <c r="E86" s="9"/>
     </row>
-    <row r="87" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C87" s="9"/>
       <c r="E87" s="9"/>
     </row>
-    <row r="88" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C88" s="9"/>
       <c r="E88" s="9"/>
     </row>
-    <row r="89" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C89" s="9"/>
       <c r="E89" s="9"/>
     </row>
-    <row r="90" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C90" s="9"/>
       <c r="E90" s="9"/>
     </row>
-    <row r="91" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C91" s="9"/>
       <c r="E91" s="9"/>
     </row>
-    <row r="92" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C92" s="9"/>
       <c r="E92" s="9"/>
     </row>
-    <row r="93" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C93" s="9"/>
       <c r="E93" s="9"/>
     </row>
-    <row r="94" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C94" s="9"/>
       <c r="E94" s="9"/>
     </row>
-    <row r="95" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C95" s="9"/>
       <c r="E95" s="9"/>
     </row>
-    <row r="96" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C96" s="9"/>
       <c r="E96" s="9"/>
     </row>
-    <row r="97" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C97" s="9"/>
       <c r="E97" s="9"/>
     </row>
-    <row r="98" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C98" s="9"/>
       <c r="E98" s="9"/>
     </row>
-    <row r="99" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C99" s="9"/>
       <c r="E99" s="9"/>
     </row>
-    <row r="100" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C100" s="9"/>
       <c r="E100" s="9"/>
     </row>
-    <row r="101" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C101" s="9"/>
       <c r="E101" s="9"/>
     </row>
-    <row r="102" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C102" s="9"/>
       <c r="E102" s="9"/>
     </row>
-    <row r="103" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C103" s="9"/>
       <c r="E103" s="9"/>
     </row>
-    <row r="104" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C104" s="9"/>
       <c r="E104" s="9"/>
     </row>
-    <row r="105" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C105" s="9"/>
       <c r="E105" s="9"/>
     </row>
-    <row r="106" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C106" s="9"/>
       <c r="E106" s="9"/>
     </row>
-    <row r="107" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C107" s="9"/>
       <c r="E107" s="9"/>
     </row>
-    <row r="108" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C108" s="9"/>
       <c r="E108" s="9"/>
     </row>
-    <row r="109" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C109" s="9"/>
       <c r="E109" s="9"/>
     </row>
-    <row r="110" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C110" s="9"/>
       <c r="E110" s="9"/>
     </row>
-    <row r="111" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C111" s="9"/>
       <c r="E111" s="9"/>
     </row>
-    <row r="112" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C112" s="9"/>
       <c r="E112" s="9"/>
     </row>
-    <row r="113" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C113" s="9"/>
       <c r="E113" s="9"/>
     </row>
-    <row r="114" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C114" s="9"/>
       <c r="E114" s="9"/>
     </row>
-    <row r="115" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C115" s="9"/>
       <c r="E115" s="9"/>
     </row>
-    <row r="116" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C116" s="9"/>
       <c r="E116" s="9"/>
     </row>
-    <row r="117" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C117" s="9"/>
       <c r="E117" s="9"/>
     </row>
-    <row r="118" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C118" s="9"/>
       <c r="E118" s="9"/>
     </row>
-    <row r="119" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C119" s="9"/>
       <c r="E119" s="9"/>
     </row>
-    <row r="120" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C120" s="9"/>
       <c r="E120" s="9"/>
     </row>
-    <row r="121" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C121" s="9"/>
       <c r="E121" s="9"/>
     </row>
-    <row r="122" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C122" s="9"/>
       <c r="E122" s="9"/>
     </row>
-    <row r="123" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C123" s="9"/>
       <c r="E123" s="9"/>
     </row>
-    <row r="124" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C124" s="9"/>
       <c r="E124" s="9"/>
     </row>
-    <row r="125" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C125" s="9"/>
       <c r="E125" s="9"/>
     </row>
-    <row r="126" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C126" s="9"/>
       <c r="E126" s="9"/>
     </row>
-    <row r="127" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C127" s="9"/>
       <c r="E127" s="9"/>
     </row>
-    <row r="128" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C128" s="9"/>
       <c r="E128" s="9"/>
     </row>
-    <row r="129" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C129" s="9"/>
       <c r="E129" s="9"/>
     </row>
-    <row r="130" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C130" s="9"/>
       <c r="E130" s="9"/>
     </row>
-    <row r="131" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C131" s="9"/>
       <c r="E131" s="9"/>
     </row>
-    <row r="132" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C132" s="9"/>
       <c r="E132" s="9"/>
     </row>
-    <row r="133" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C133" s="9"/>
       <c r="E133" s="9"/>
     </row>
-    <row r="134" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C134" s="9"/>
       <c r="E134" s="9"/>
     </row>
-    <row r="135" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C135" s="9"/>
       <c r="E135" s="9"/>
     </row>
-    <row r="136" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C136" s="9"/>
       <c r="E136" s="9"/>
     </row>
-    <row r="137" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C137" s="9"/>
       <c r="E137" s="9"/>
     </row>
-    <row r="138" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C138" s="9"/>
       <c r="E138" s="9"/>
     </row>
-    <row r="139" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C139" s="9"/>
       <c r="E139" s="9"/>
     </row>
-    <row r="140" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C140" s="9"/>
       <c r="E140" s="9"/>
     </row>
-    <row r="141" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C141" s="9"/>
       <c r="E141" s="9"/>
     </row>
-    <row r="142" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C142" s="9"/>
       <c r="E142" s="9"/>
     </row>
-    <row r="143" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C143" s="9"/>
       <c r="E143" s="9"/>
     </row>
-    <row r="144" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C144" s="9"/>
       <c r="E144" s="9"/>
     </row>
-    <row r="145" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C145" s="9"/>
       <c r="E145" s="9"/>
     </row>
-    <row r="146" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C146" s="9"/>
       <c r="E146" s="9"/>
     </row>
-    <row r="147" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C147" s="9"/>
       <c r="E147" s="9"/>
     </row>
-    <row r="148" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C148" s="9"/>
       <c r="E148" s="9"/>
     </row>
-    <row r="149" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C149" s="9"/>
       <c r="E149" s="9"/>
     </row>
-    <row r="150" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C150" s="9"/>
       <c r="E150" s="9"/>
     </row>
-    <row r="151" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C151" s="9"/>
       <c r="E151" s="9"/>
     </row>
-    <row r="152" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C152" s="9"/>
       <c r="E152" s="9"/>
     </row>
-    <row r="153" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C153" s="9"/>
       <c r="E153" s="9"/>
     </row>
-    <row r="154" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C154" s="9"/>
       <c r="E154" s="9"/>
     </row>
-    <row r="155" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C155" s="9"/>
       <c r="E155" s="9"/>
     </row>
-    <row r="156" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C156" s="9"/>
       <c r="E156" s="9"/>
     </row>
-    <row r="157" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C157" s="9"/>
       <c r="E157" s="9"/>
     </row>
-    <row r="158" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C158" s="9"/>
       <c r="E158" s="9"/>
     </row>
-    <row r="159" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C159" s="9"/>
       <c r="E159" s="9"/>
     </row>
-    <row r="160" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C160" s="9"/>
       <c r="E160" s="9"/>
     </row>
-    <row r="161" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C161" s="9"/>
       <c r="E161" s="9"/>
     </row>
-    <row r="162" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C162" s="9"/>
       <c r="E162" s="9"/>
     </row>
-    <row r="163" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C163" s="9"/>
       <c r="E163" s="9"/>
     </row>
-    <row r="164" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C164" s="9"/>
       <c r="E164" s="9"/>
     </row>
-    <row r="165" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C165" s="9"/>
       <c r="E165" s="9"/>
     </row>
-    <row r="166" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C166" s="9"/>
       <c r="E166" s="9"/>
     </row>
-    <row r="167" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C167" s="9"/>
       <c r="E167" s="9"/>
     </row>
-    <row r="168" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C168" s="9"/>
       <c r="E168" s="9"/>
     </row>
-    <row r="169" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C169" s="9"/>
       <c r="E169" s="9"/>
     </row>
-    <row r="170" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C170" s="9"/>
       <c r="E170" s="9"/>
     </row>
-    <row r="171" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C171" s="9"/>
       <c r="E171" s="9"/>
     </row>
-    <row r="172" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C172" s="9"/>
       <c r="E172" s="9"/>
     </row>
-    <row r="173" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C173" s="9"/>
       <c r="E173" s="9"/>
     </row>
-    <row r="174" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C174" s="9"/>
       <c r="E174" s="9"/>
     </row>
-    <row r="175" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C175" s="9"/>
       <c r="E175" s="9"/>
     </row>
-    <row r="176" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C176" s="9"/>
       <c r="E176" s="9"/>
     </row>
-    <row r="177" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C177" s="9"/>
       <c r="E177" s="9"/>
     </row>
-    <row r="178" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C178" s="9"/>
       <c r="E178" s="9"/>
     </row>
-    <row r="179" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C179" s="9"/>
       <c r="E179" s="9"/>
     </row>
-    <row r="180" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C180" s="9"/>
       <c r="E180" s="9"/>
     </row>
-    <row r="181" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C181" s="9"/>
       <c r="E181" s="9"/>
     </row>
-    <row r="182" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C182" s="9"/>
       <c r="E182" s="9"/>
     </row>
-    <row r="183" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C183" s="9"/>
       <c r="E183" s="9"/>
     </row>
-    <row r="184" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C184" s="9"/>
       <c r="E184" s="9"/>
     </row>
-    <row r="185" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C185" s="9"/>
       <c r="E185" s="9"/>
     </row>
-    <row r="186" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C186" s="9"/>
       <c r="E186" s="9"/>
     </row>
-    <row r="187" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C187" s="9"/>
       <c r="E187" s="9"/>
     </row>
-    <row r="188" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C188" s="9"/>
       <c r="E188" s="9"/>
     </row>
-    <row r="189" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C189" s="9"/>
       <c r="E189" s="9"/>
     </row>
-    <row r="190" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C190" s="9"/>
       <c r="E190" s="9"/>
     </row>
-    <row r="191" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C191" s="9"/>
       <c r="E191" s="9"/>
     </row>
-    <row r="192" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C192" s="9"/>
       <c r="E192" s="9"/>
     </row>
-    <row r="193" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C193" s="9"/>
       <c r="E193" s="9"/>
     </row>
-    <row r="194" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C194" s="9"/>
       <c r="E194" s="9"/>
     </row>
-    <row r="195" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C195" s="9"/>
       <c r="E195" s="9"/>
     </row>
-    <row r="196" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C196" s="9"/>
       <c r="E196" s="9"/>
     </row>
-    <row r="197" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C197" s="9"/>
       <c r="E197" s="9"/>
     </row>
-    <row r="198" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C198" s="9"/>
       <c r="E198" s="9"/>
     </row>
-    <row r="199" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C199" s="9"/>
       <c r="E199" s="9"/>
     </row>
-    <row r="200" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C200" s="9"/>
       <c r="E200" s="9"/>
     </row>
-    <row r="201" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C201" s="9"/>
       <c r="E201" s="9"/>
     </row>
-    <row r="202" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C202" s="9"/>
       <c r="E202" s="9"/>
     </row>
-    <row r="203" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C203" s="9"/>
       <c r="E203" s="9"/>
     </row>
-    <row r="204" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C204" s="9"/>
       <c r="E204" s="9"/>
     </row>
-    <row r="205" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C205" s="9"/>
       <c r="E205" s="9"/>
     </row>
-    <row r="206" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C206" s="9"/>
       <c r="E206" s="9"/>
     </row>
-    <row r="207" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C207" s="9"/>
       <c r="E207" s="9"/>
     </row>
-    <row r="208" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C208" s="9"/>
       <c r="E208" s="9"/>
     </row>
-    <row r="209" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C209" s="9"/>
       <c r="E209" s="9"/>
     </row>
-    <row r="210" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C210" s="9"/>
       <c r="E210" s="9"/>
     </row>
-    <row r="211" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C211" s="9"/>
       <c r="E211" s="9"/>
     </row>
-    <row r="212" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C212" s="9"/>
       <c r="E212" s="9"/>
     </row>
-    <row r="213" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C213" s="9"/>
       <c r="E213" s="9"/>
     </row>
-    <row r="214" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C214" s="9"/>
       <c r="E214" s="9"/>
     </row>
-    <row r="215" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C215" s="9"/>
       <c r="E215" s="9"/>
     </row>
-    <row r="216" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C216" s="9"/>
       <c r="E216" s="9"/>
     </row>
-    <row r="217" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C217" s="9"/>
       <c r="E217" s="9"/>
     </row>
-    <row r="218" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C218" s="9"/>
       <c r="E218" s="9"/>
     </row>
-    <row r="219" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C219" s="9"/>
       <c r="E219" s="9"/>
     </row>
-    <row r="220" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C220" s="9"/>
       <c r="E220" s="9"/>
     </row>
-    <row r="221" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C221" s="9"/>
       <c r="E221" s="9"/>
     </row>
-    <row r="222" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C222" s="9"/>
       <c r="E222" s="9"/>
     </row>
-    <row r="223" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C223" s="9"/>
       <c r="E223" s="9"/>
     </row>
-    <row r="224" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C224" s="9"/>
       <c r="E224" s="9"/>
     </row>
-    <row r="225" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="225" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C225" s="9"/>
       <c r="E225" s="9"/>
     </row>
-    <row r="226" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="226" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C226" s="9"/>
       <c r="E226" s="9"/>
     </row>
-    <row r="227" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C227" s="9"/>
       <c r="E227" s="9"/>
     </row>
-    <row r="228" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="228" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C228" s="9"/>
       <c r="E228" s="9"/>
     </row>
-    <row r="229" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="229" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C229" s="9"/>
       <c r="E229" s="9"/>
     </row>
-    <row r="230" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="230" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C230" s="9"/>
       <c r="E230" s="9"/>
     </row>
-    <row r="231" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="231" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C231" s="9"/>
       <c r="E231" s="9"/>
     </row>
-    <row r="232" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="232" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C232" s="9"/>
       <c r="E232" s="9"/>
     </row>
-    <row r="233" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="233" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C233" s="9"/>
       <c r="E233" s="9"/>
     </row>
-    <row r="234" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C234" s="9"/>
       <c r="E234" s="9"/>
     </row>
-    <row r="235" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C235" s="9"/>
       <c r="E235" s="9"/>
     </row>
-    <row r="236" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C236" s="9"/>
       <c r="E236" s="9"/>
     </row>
-    <row r="237" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C237" s="9"/>
       <c r="E237" s="9"/>
     </row>
-    <row r="238" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C238" s="9"/>
       <c r="E238" s="9"/>
     </row>
-    <row r="239" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C239" s="9"/>
       <c r="E239" s="9"/>
     </row>
-    <row r="240" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C240" s="9"/>
       <c r="E240" s="9"/>
     </row>
-    <row r="241" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="241" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C241" s="9"/>
       <c r="E241" s="9"/>
     </row>
-    <row r="242" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="242" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C242" s="9"/>
       <c r="E242" s="9"/>
     </row>
-    <row r="243" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="243" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C243" s="9"/>
       <c r="E243" s="9"/>
     </row>
-    <row r="244" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="244" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C244" s="9"/>
       <c r="E244" s="9"/>
     </row>
-    <row r="245" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="245" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C245" s="9"/>
       <c r="E245" s="9"/>
     </row>
-    <row r="246" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="246" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C246" s="9"/>
       <c r="E246" s="9"/>
     </row>
-    <row r="247" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="247" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C247" s="9"/>
       <c r="E247" s="9"/>
     </row>
-    <row r="248" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="248" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C248" s="9"/>
       <c r="E248" s="9"/>
     </row>
-    <row r="249" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="249" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C249" s="9"/>
       <c r="E249" s="9"/>
     </row>
-    <row r="250" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="250" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C250" s="9"/>
       <c r="E250" s="9"/>
     </row>
-    <row r="251" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="251" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C251" s="9"/>
       <c r="E251" s="9"/>
     </row>
-    <row r="252" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="252" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C252" s="9"/>
       <c r="E252" s="9"/>
     </row>
-    <row r="253" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="253" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C253" s="9"/>
       <c r="E253" s="9"/>
     </row>
-    <row r="254" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="254" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C254" s="9"/>
       <c r="E254" s="9"/>
     </row>
-    <row r="255" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="255" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C255" s="9"/>
       <c r="E255" s="9"/>
     </row>
-    <row r="256" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="256" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C256" s="9"/>
       <c r="E256" s="9"/>
     </row>
-    <row r="257" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="257" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C257" s="9"/>
       <c r="E257" s="9"/>
     </row>
-    <row r="258" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="258" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C258" s="9"/>
       <c r="E258" s="9"/>
     </row>
-    <row r="259" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="259" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C259" s="9"/>
       <c r="E259" s="9"/>
     </row>
-    <row r="260" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="260" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C260" s="9"/>
       <c r="E260" s="9"/>
     </row>
-    <row r="261" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="261" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C261" s="9"/>
       <c r="E261" s="9"/>
     </row>
-    <row r="262" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="262" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C262" s="9"/>
       <c r="E262" s="9"/>
     </row>
-    <row r="263" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="263" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C263" s="9"/>
       <c r="E263" s="9"/>
     </row>
-    <row r="264" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="264" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C264" s="9"/>
       <c r="E264" s="9"/>
     </row>
-    <row r="265" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="265" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C265" s="9"/>
       <c r="E265" s="9"/>
     </row>
-    <row r="266" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="266" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C266" s="9"/>
       <c r="E266" s="9"/>
     </row>
-    <row r="267" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="267" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C267" s="9"/>
       <c r="E267" s="9"/>
     </row>
-    <row r="268" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="268" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C268" s="9"/>
       <c r="E268" s="9"/>
     </row>
-    <row r="269" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="269" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C269" s="9"/>
       <c r="E269" s="9"/>
     </row>
-    <row r="270" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="270" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C270" s="9"/>
       <c r="E270" s="9"/>
     </row>
-    <row r="271" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="271" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C271" s="9"/>
       <c r="E271" s="9"/>
     </row>
-    <row r="272" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="272" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C272" s="9"/>
       <c r="E272" s="9"/>
     </row>
-    <row r="273" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="273" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C273" s="9"/>
       <c r="E273" s="9"/>
     </row>
-    <row r="274" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="274" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C274" s="9"/>
       <c r="E274" s="9"/>
     </row>
-    <row r="275" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="275" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C275" s="9"/>
       <c r="E275" s="9"/>
     </row>
-    <row r="276" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="276" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C276" s="9"/>
       <c r="E276" s="9"/>
     </row>
-    <row r="277" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="277" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C277" s="9"/>
       <c r="E277" s="9"/>
     </row>
-    <row r="278" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="278" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C278" s="9"/>
       <c r="E278" s="9"/>
     </row>
-    <row r="279" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="279" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C279" s="9"/>
       <c r="E279" s="9"/>
     </row>
-    <row r="280" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="280" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C280" s="9"/>
       <c r="E280" s="9"/>
     </row>
-    <row r="281" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="281" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C281" s="9"/>
       <c r="E281" s="9"/>
     </row>
-    <row r="282" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="282" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C282" s="9"/>
       <c r="E282" s="9"/>
     </row>
-    <row r="283" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C283" s="9"/>
       <c r="E283" s="9"/>
     </row>
-    <row r="284" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="284" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C284" s="9"/>
       <c r="E284" s="9"/>
     </row>
-    <row r="285" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="285" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C285" s="9"/>
       <c r="E285" s="9"/>
     </row>
-    <row r="286" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="286" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C286" s="9"/>
       <c r="E286" s="9"/>
     </row>
-    <row r="287" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="287" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C287" s="9"/>
       <c r="E287" s="9"/>
     </row>
-    <row r="288" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="288" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C288" s="9"/>
       <c r="E288" s="9"/>
     </row>
-    <row r="289" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="289" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C289" s="9"/>
       <c r="E289" s="9"/>
     </row>
-    <row r="290" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="290" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C290" s="9"/>
       <c r="E290" s="9"/>
     </row>
-    <row r="291" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="291" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C291" s="9"/>
       <c r="E291" s="9"/>
     </row>
-    <row r="292" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="292" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C292" s="9"/>
       <c r="E292" s="9"/>
     </row>
-    <row r="293" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="293" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C293" s="9"/>
       <c r="E293" s="9"/>
     </row>
-    <row r="294" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="294" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C294" s="9"/>
       <c r="E294" s="9"/>
     </row>
-    <row r="295" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="295" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C295" s="9"/>
       <c r="E295" s="9"/>
     </row>
-    <row r="296" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="296" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C296" s="9"/>
       <c r="E296" s="9"/>
     </row>
-    <row r="297" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="297" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C297" s="9"/>
       <c r="E297" s="9"/>
     </row>
-    <row r="298" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="298" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C298" s="9"/>
       <c r="E298" s="9"/>
     </row>
-    <row r="299" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="299" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C299" s="9"/>
       <c r="E299" s="9"/>
     </row>
-    <row r="300" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="300" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C300" s="9"/>
       <c r="E300" s="9"/>
     </row>
-    <row r="301" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="301" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C301" s="9"/>
       <c r="E301" s="9"/>
     </row>
-    <row r="302" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="302" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C302" s="9"/>
       <c r="E302" s="9"/>
     </row>
-    <row r="303" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="303" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C303" s="9"/>
       <c r="E303" s="9"/>
     </row>
-    <row r="304" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="304" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C304" s="9"/>
       <c r="E304" s="9"/>
     </row>
-    <row r="305" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="305" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C305" s="9"/>
       <c r="E305" s="9"/>
     </row>
-    <row r="306" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="306" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C306" s="9"/>
       <c r="E306" s="9"/>
     </row>
-    <row r="307" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="307" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C307" s="9"/>
       <c r="E307" s="9"/>
     </row>
-    <row r="308" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="308" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C308" s="9"/>
       <c r="E308" s="9"/>
     </row>
-    <row r="309" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="309" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C309" s="9"/>
       <c r="E309" s="9"/>
     </row>
-    <row r="310" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="310" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C310" s="9"/>
       <c r="E310" s="9"/>
     </row>
-    <row r="311" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="311" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C311" s="9"/>
       <c r="E311" s="9"/>
     </row>
-    <row r="312" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="312" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C312" s="9"/>
       <c r="E312" s="9"/>
     </row>
-    <row r="313" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="313" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C313" s="9"/>
       <c r="E313" s="9"/>
     </row>
-    <row r="314" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="314" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C314" s="9"/>
       <c r="E314" s="9"/>
     </row>
-    <row r="315" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="315" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C315" s="9"/>
       <c r="E315" s="9"/>
     </row>
-    <row r="316" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="316" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C316" s="9"/>
       <c r="E316" s="9"/>
     </row>
-    <row r="317" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="317" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C317" s="9"/>
       <c r="E317" s="9"/>
     </row>
-    <row r="318" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="318" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C318" s="9"/>
       <c r="E318" s="9"/>
     </row>
-    <row r="319" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="319" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C319" s="9"/>
       <c r="E319" s="9"/>
     </row>
-    <row r="320" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="320" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C320" s="9"/>
       <c r="E320" s="9"/>
     </row>
-    <row r="321" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="321" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C321" s="9"/>
       <c r="E321" s="9"/>
     </row>
-    <row r="322" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="322" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C322" s="9"/>
       <c r="E322" s="9"/>
     </row>
-    <row r="323" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="323" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C323" s="9"/>
       <c r="E323" s="9"/>
     </row>
-    <row r="324" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="324" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C324" s="9"/>
       <c r="E324" s="9"/>
     </row>
-    <row r="325" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="325" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C325" s="9"/>
       <c r="E325" s="9"/>
     </row>
-    <row r="326" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="326" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C326" s="9"/>
       <c r="E326" s="9"/>
     </row>
-    <row r="327" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="327" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C327" s="9"/>
       <c r="E327" s="9"/>
     </row>
-    <row r="328" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="328" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C328" s="9"/>
       <c r="E328" s="9"/>
     </row>
-    <row r="329" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="329" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C329" s="9"/>
       <c r="E329" s="9"/>
     </row>
-    <row r="330" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="330" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C330" s="9"/>
       <c r="E330" s="9"/>
     </row>
-    <row r="331" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="331" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C331" s="9"/>
       <c r="E331" s="9"/>
     </row>
-    <row r="332" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="332" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C332" s="9"/>
       <c r="E332" s="9"/>
     </row>
-    <row r="333" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="333" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C333" s="9"/>
       <c r="E333" s="9"/>
     </row>
-    <row r="334" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="334" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C334" s="9"/>
       <c r="E334" s="9"/>
     </row>
-    <row r="335" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="335" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C335" s="9"/>
       <c r="E335" s="9"/>
     </row>
-    <row r="336" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="336" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C336" s="9"/>
       <c r="E336" s="9"/>
     </row>
-    <row r="337" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="337" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C337" s="9"/>
       <c r="E337" s="9"/>
     </row>
-    <row r="338" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="338" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C338" s="9"/>
       <c r="E338" s="9"/>
     </row>
-    <row r="339" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="339" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C339" s="9"/>
       <c r="E339" s="9"/>
     </row>
-    <row r="340" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="340" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C340" s="9"/>
       <c r="E340" s="9"/>
     </row>
-    <row r="341" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="341" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C341" s="9"/>
       <c r="E341" s="9"/>
     </row>
-    <row r="342" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="342" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C342" s="9"/>
       <c r="E342" s="9"/>
     </row>
-    <row r="343" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="343" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C343" s="9"/>
       <c r="E343" s="9"/>
     </row>
-    <row r="344" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="344" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C344" s="9"/>
       <c r="E344" s="9"/>
     </row>
-    <row r="345" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="345" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C345" s="9"/>
       <c r="E345" s="9"/>
     </row>
-    <row r="346" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="346" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C346" s="9"/>
       <c r="E346" s="9"/>
     </row>
-    <row r="347" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="347" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C347" s="9"/>
       <c r="E347" s="9"/>
     </row>
-    <row r="348" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="348" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C348" s="9"/>
       <c r="E348" s="9"/>
     </row>
-    <row r="349" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="349" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C349" s="9"/>
       <c r="E349" s="9"/>
     </row>
-    <row r="350" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="350" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C350" s="9"/>
       <c r="E350" s="9"/>
     </row>
-    <row r="351" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="351" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C351" s="9"/>
       <c r="E351" s="9"/>
     </row>
-    <row r="352" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="352" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C352" s="9"/>
       <c r="E352" s="9"/>
     </row>
-    <row r="353" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="353" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C353" s="9"/>
       <c r="E353" s="9"/>
     </row>
-    <row r="354" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="354" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C354" s="9"/>
       <c r="E354" s="9"/>
     </row>
-    <row r="355" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="355" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C355" s="9"/>
       <c r="E355" s="9"/>
     </row>
-    <row r="356" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="356" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C356" s="9"/>
       <c r="E356" s="9"/>
     </row>
-    <row r="357" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="357" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C357" s="9"/>
       <c r="E357" s="9"/>
     </row>
-    <row r="358" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="358" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C358" s="9"/>
       <c r="E358" s="9"/>
     </row>
-    <row r="359" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="359" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C359" s="9"/>
       <c r="E359" s="9"/>
     </row>
-    <row r="360" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="360" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C360" s="9"/>
       <c r="E360" s="9"/>
     </row>
-    <row r="361" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="361" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C361" s="9"/>
       <c r="E361" s="9"/>
     </row>
-    <row r="362" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="362" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C362" s="9"/>
       <c r="E362" s="9"/>
     </row>
-    <row r="363" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="363" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C363" s="9"/>
       <c r="E363" s="9"/>
     </row>
-    <row r="364" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="364" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C364" s="9"/>
       <c r="E364" s="9"/>
     </row>
-    <row r="365" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="365" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C365" s="9"/>
       <c r="E365" s="9"/>
     </row>
-    <row r="366" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="366" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C366" s="9"/>
       <c r="E366" s="9"/>
     </row>
-    <row r="367" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="367" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C367" s="9"/>
       <c r="E367" s="9"/>
     </row>
-    <row r="368" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="368" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C368" s="9"/>
       <c r="E368" s="9"/>
     </row>
-    <row r="369" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="369" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C369" s="9"/>
       <c r="E369" s="9"/>
     </row>
-    <row r="370" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="370" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C370" s="9"/>
       <c r="E370" s="9"/>
     </row>
-    <row r="371" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="371" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C371" s="9"/>
       <c r="E371" s="9"/>
     </row>
-    <row r="372" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="372" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C372" s="9"/>
       <c r="E372" s="9"/>
     </row>
-    <row r="373" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="373" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C373" s="9"/>
       <c r="E373" s="9"/>
     </row>
-    <row r="374" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="374" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C374" s="9"/>
       <c r="E374" s="9"/>
     </row>
-    <row r="375" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="375" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C375" s="9"/>
       <c r="E375" s="9"/>
     </row>
-    <row r="376" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="376" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C376" s="9"/>
       <c r="E376" s="9"/>
     </row>
-    <row r="377" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="377" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C377" s="9"/>
       <c r="E377" s="9"/>
     </row>
-    <row r="378" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="378" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C378" s="9"/>
       <c r="E378" s="9"/>
     </row>
-    <row r="379" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="379" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C379" s="9"/>
       <c r="E379" s="9"/>
     </row>
-    <row r="380" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="380" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C380" s="9"/>
       <c r="E380" s="9"/>
     </row>
-    <row r="381" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="381" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C381" s="9"/>
       <c r="E381" s="9"/>
     </row>
-    <row r="382" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="382" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C382" s="9"/>
       <c r="E382" s="9"/>
     </row>
-    <row r="383" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="383" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C383" s="9"/>
       <c r="E383" s="9"/>
     </row>
-    <row r="384" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="384" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C384" s="9"/>
       <c r="E384" s="9"/>
     </row>
-    <row r="385" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="385" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C385" s="9"/>
       <c r="E385" s="9"/>
     </row>
-    <row r="386" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="386" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C386" s="9"/>
       <c r="E386" s="9"/>
     </row>
-    <row r="387" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="387" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C387" s="9"/>
       <c r="E387" s="9"/>
     </row>
-    <row r="388" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="388" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C388" s="9"/>
       <c r="E388" s="9"/>
     </row>
-    <row r="389" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="389" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C389" s="9"/>
       <c r="E389" s="9"/>
     </row>
-    <row r="390" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="390" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C390" s="9"/>
       <c r="E390" s="9"/>
     </row>
-    <row r="391" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="391" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C391" s="9"/>
       <c r="E391" s="9"/>
     </row>
-    <row r="392" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="392" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C392" s="9"/>
       <c r="E392" s="9"/>
     </row>
-    <row r="393" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="393" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C393" s="9"/>
       <c r="E393" s="9"/>
     </row>
-    <row r="394" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="394" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C394" s="9"/>
       <c r="E394" s="9"/>
     </row>
-    <row r="395" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="395" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C395" s="9"/>
       <c r="E395" s="9"/>
     </row>
-    <row r="396" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="396" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C396" s="9"/>
       <c r="E396" s="9"/>
     </row>
-    <row r="397" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="397" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C397" s="9"/>
       <c r="E397" s="9"/>
     </row>
-    <row r="398" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="398" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C398" s="9"/>
       <c r="E398" s="9"/>
     </row>
-    <row r="399" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="399" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C399" s="9"/>
       <c r="E399" s="9"/>
     </row>
-    <row r="400" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="400" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C400" s="9"/>
       <c r="E400" s="9"/>
     </row>
-    <row r="401" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="401" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C401" s="9"/>
       <c r="E401" s="9"/>
     </row>
-    <row r="402" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="402" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C402" s="9"/>
       <c r="E402" s="9"/>
     </row>
-    <row r="403" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="403" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C403" s="9"/>
       <c r="E403" s="9"/>
     </row>
-    <row r="404" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="404" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C404" s="9"/>
       <c r="E404" s="9"/>
     </row>
-    <row r="405" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="405" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C405" s="9"/>
       <c r="E405" s="9"/>
     </row>
-    <row r="406" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="406" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C406" s="9"/>
       <c r="E406" s="9"/>
     </row>
-    <row r="407" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="407" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C407" s="9"/>
       <c r="E407" s="9"/>
     </row>
-    <row r="408" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="408" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C408" s="9"/>
       <c r="E408" s="9"/>
     </row>
-    <row r="409" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="409" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C409" s="9"/>
       <c r="E409" s="9"/>
     </row>
-    <row r="410" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="410" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C410" s="9"/>
       <c r="E410" s="9"/>
     </row>
-    <row r="411" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="411" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C411" s="9"/>
       <c r="E411" s="9"/>
     </row>
-    <row r="412" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="412" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C412" s="9"/>
       <c r="E412" s="9"/>
     </row>
-    <row r="413" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="413" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C413" s="9"/>
       <c r="E413" s="9"/>
     </row>
-    <row r="414" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="414" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C414" s="9"/>
       <c r="E414" s="9"/>
     </row>
-    <row r="415" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="415" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C415" s="9"/>
       <c r="E415" s="9"/>
     </row>
-    <row r="416" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="416" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C416" s="9"/>
       <c r="E416" s="9"/>
     </row>
-    <row r="417" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="417" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C417" s="9"/>
       <c r="E417" s="9"/>
     </row>
-    <row r="418" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="418" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C418" s="9"/>
       <c r="E418" s="9"/>
     </row>
-    <row r="419" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="419" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C419" s="9"/>
       <c r="E419" s="9"/>
     </row>
-    <row r="420" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="420" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C420" s="9"/>
       <c r="E420" s="9"/>
     </row>
-    <row r="421" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="421" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C421" s="9"/>
       <c r="E421" s="9"/>
     </row>
-    <row r="422" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="422" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C422" s="9"/>
       <c r="E422" s="9"/>
     </row>
-    <row r="423" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="423" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C423" s="9"/>
       <c r="E423" s="9"/>
     </row>
-    <row r="424" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="424" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C424" s="9"/>
       <c r="E424" s="9"/>
     </row>
-    <row r="425" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="425" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C425" s="9"/>
       <c r="E425" s="9"/>
     </row>
-    <row r="426" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="426" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C426" s="9"/>
       <c r="E426" s="9"/>
     </row>
-    <row r="427" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="427" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C427" s="9"/>
       <c r="E427" s="9"/>
     </row>
-    <row r="428" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="428" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C428" s="9"/>
       <c r="E428" s="9"/>
     </row>
-    <row r="429" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="429" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C429" s="9"/>
       <c r="E429" s="9"/>
     </row>
-    <row r="430" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="430" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C430" s="9"/>
       <c r="E430" s="9"/>
     </row>
-    <row r="431" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="431" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C431" s="9"/>
       <c r="E431" s="9"/>
     </row>
-    <row r="432" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="432" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C432" s="9"/>
       <c r="E432" s="9"/>
     </row>
-    <row r="433" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="433" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C433" s="9"/>
       <c r="E433" s="9"/>
     </row>
-    <row r="434" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="434" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C434" s="9"/>
       <c r="E434" s="9"/>
     </row>
-    <row r="435" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="435" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C435" s="9"/>
       <c r="E435" s="9"/>
     </row>
-    <row r="436" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="436" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C436" s="9"/>
       <c r="E436" s="9"/>
     </row>
-    <row r="437" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="437" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C437" s="9"/>
       <c r="E437" s="9"/>
     </row>
-    <row r="438" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="438" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C438" s="9"/>
       <c r="E438" s="9"/>
     </row>
-    <row r="439" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="439" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C439" s="9"/>
       <c r="E439" s="9"/>
     </row>
-    <row r="440" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="440" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C440" s="9"/>
       <c r="E440" s="9"/>
     </row>
-    <row r="441" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="441" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C441" s="9"/>
       <c r="E441" s="9"/>
     </row>
-    <row r="442" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="442" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C442" s="9"/>
       <c r="E442" s="9"/>
     </row>
-    <row r="443" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="443" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C443" s="9"/>
       <c r="E443" s="9"/>
     </row>
-    <row r="444" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="444" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C444" s="9"/>
       <c r="E444" s="9"/>
     </row>
-    <row r="445" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="445" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C445" s="9"/>
       <c r="E445" s="9"/>
     </row>
-    <row r="446" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="446" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C446" s="9"/>
       <c r="E446" s="9"/>
     </row>
-    <row r="447" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="447" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C447" s="9"/>
       <c r="E447" s="9"/>
     </row>
-    <row r="448" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="448" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C448" s="9"/>
       <c r="E448" s="9"/>
     </row>
-    <row r="449" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="449" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C449" s="9"/>
       <c r="E449" s="9"/>
     </row>
-    <row r="450" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="450" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C450" s="9"/>
       <c r="E450" s="9"/>
     </row>
-    <row r="451" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="451" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C451" s="9"/>
       <c r="E451" s="9"/>
     </row>
-    <row r="452" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="452" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C452" s="9"/>
       <c r="E452" s="9"/>
     </row>
-    <row r="453" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="453" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C453" s="9"/>
       <c r="E453" s="9"/>
     </row>
-    <row r="454" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="454" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C454" s="9"/>
       <c r="E454" s="9"/>
     </row>
-    <row r="455" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="455" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C455" s="9"/>
       <c r="E455" s="9"/>
     </row>
-    <row r="456" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="456" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C456" s="9"/>
       <c r="E456" s="9"/>
     </row>
-    <row r="457" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="457" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C457" s="9"/>
       <c r="E457" s="9"/>
     </row>
-    <row r="458" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="458" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C458" s="9"/>
       <c r="E458" s="9"/>
     </row>
-    <row r="459" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="459" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C459" s="9"/>
       <c r="E459" s="9"/>
     </row>
-    <row r="460" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="460" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C460" s="9"/>
       <c r="E460" s="9"/>
     </row>
-    <row r="461" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="461" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C461" s="9"/>
       <c r="E461" s="9"/>
     </row>
-    <row r="462" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="462" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C462" s="9"/>
       <c r="E462" s="9"/>
     </row>
-    <row r="463" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="463" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C463" s="9"/>
       <c r="E463" s="9"/>
     </row>
-    <row r="464" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="464" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C464" s="9"/>
       <c r="E464" s="9"/>
     </row>
-    <row r="465" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="465" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C465" s="9"/>
       <c r="E465" s="9"/>
     </row>
-    <row r="466" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="466" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C466" s="9"/>
       <c r="E466" s="9"/>
     </row>
-    <row r="467" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="467" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C467" s="9"/>
       <c r="E467" s="9"/>
     </row>
-    <row r="468" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="468" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C468" s="9"/>
       <c r="E468" s="9"/>
     </row>
-    <row r="469" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="469" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C469" s="9"/>
       <c r="E469" s="9"/>
     </row>
-    <row r="470" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="470" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C470" s="9"/>
       <c r="E470" s="9"/>
     </row>
-    <row r="471" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="471" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C471" s="9"/>
       <c r="E471" s="9"/>
     </row>
-    <row r="472" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="472" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C472" s="9"/>
       <c r="E472" s="9"/>
     </row>
-    <row r="473" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="473" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C473" s="9"/>
       <c r="E473" s="9"/>
     </row>
-    <row r="474" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="474" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C474" s="9"/>
       <c r="E474" s="9"/>
     </row>
-    <row r="475" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="475" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C475" s="9"/>
       <c r="E475" s="9"/>
     </row>
-    <row r="476" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="476" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C476" s="9"/>
       <c r="E476" s="9"/>
     </row>
-    <row r="477" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="477" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C477" s="9"/>
       <c r="E477" s="9"/>
     </row>
-    <row r="478" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="478" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C478" s="9"/>
       <c r="E478" s="9"/>
     </row>
-    <row r="479" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="479" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C479" s="9"/>
       <c r="E479" s="9"/>
     </row>
-    <row r="480" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="480" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C480" s="9"/>
       <c r="E480" s="9"/>
     </row>
-    <row r="481" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="481" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C481" s="9"/>
       <c r="E481" s="9"/>
     </row>
-    <row r="482" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="482" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C482" s="9"/>
       <c r="E482" s="9"/>
     </row>
-    <row r="483" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="483" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C483" s="9"/>
       <c r="E483" s="9"/>
     </row>
-    <row r="484" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="484" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C484" s="9"/>
       <c r="E484" s="9"/>
     </row>
-    <row r="485" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="485" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C485" s="9"/>
       <c r="E485" s="9"/>
     </row>
-    <row r="486" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="486" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C486" s="9"/>
       <c r="E486" s="9"/>
     </row>
-    <row r="487" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="487" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C487" s="9"/>
       <c r="E487" s="9"/>
     </row>
-    <row r="488" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="488" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C488" s="9"/>
       <c r="E488" s="9"/>
     </row>
-    <row r="489" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="489" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C489" s="9"/>
       <c r="E489" s="9"/>
     </row>
-    <row r="490" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="490" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C490" s="9"/>
       <c r="E490" s="9"/>
     </row>
-    <row r="491" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="491" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C491" s="9"/>
       <c r="E491" s="9"/>
     </row>
-    <row r="492" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="492" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C492" s="9"/>
       <c r="E492" s="9"/>
     </row>
-    <row r="493" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="493" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C493" s="9"/>
       <c r="E493" s="9"/>
     </row>
-    <row r="494" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="494" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C494" s="9"/>
       <c r="E494" s="9"/>
     </row>
-    <row r="495" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="495" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C495" s="9"/>
       <c r="E495" s="9"/>
     </row>
-    <row r="496" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="496" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C496" s="9"/>
       <c r="E496" s="9"/>
     </row>
-    <row r="497" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="497" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C497" s="9"/>
       <c r="E497" s="9"/>
     </row>
-    <row r="498" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="498" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C498" s="9"/>
       <c r="E498" s="9"/>
     </row>
-    <row r="499" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="499" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C499" s="9"/>
       <c r="E499" s="9"/>
     </row>
-    <row r="500" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="500" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C500" s="9"/>
       <c r="E500" s="9"/>
     </row>
-    <row r="501" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="501" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C501" s="9"/>
       <c r="E501" s="9"/>
     </row>
-    <row r="502" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="502" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C502" s="9"/>
       <c r="E502" s="9"/>
     </row>
-    <row r="503" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="503" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C503" s="9"/>
       <c r="E503" s="9"/>
     </row>
-    <row r="504" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="504" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C504" s="9"/>
       <c r="E504" s="9"/>
     </row>
-    <row r="505" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="505" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C505" s="9"/>
       <c r="E505" s="9"/>
     </row>
-    <row r="506" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="506" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C506" s="9"/>
       <c r="E506" s="9"/>
     </row>
-    <row r="507" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="507" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C507" s="9"/>
       <c r="E507" s="9"/>
     </row>
-    <row r="508" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="508" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C508" s="9"/>
       <c r="E508" s="9"/>
     </row>
-    <row r="509" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="509" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C509" s="9"/>
       <c r="E509" s="9"/>
     </row>
-    <row r="510" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="510" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C510" s="9"/>
       <c r="E510" s="9"/>
     </row>
-    <row r="511" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="511" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C511" s="9"/>
       <c r="E511" s="9"/>
     </row>
-    <row r="512" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="512" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C512" s="9"/>
       <c r="E512" s="9"/>
     </row>
-    <row r="513" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="513" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C513" s="9"/>
       <c r="E513" s="9"/>
     </row>
-    <row r="514" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="514" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C514" s="9"/>
       <c r="E514" s="9"/>
     </row>
-    <row r="515" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="515" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C515" s="9"/>
       <c r="E515" s="9"/>
     </row>
-    <row r="516" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="516" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C516" s="9"/>
       <c r="E516" s="9"/>
     </row>
-    <row r="517" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="517" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C517" s="9"/>
       <c r="E517" s="9"/>
     </row>
-    <row r="518" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="518" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C518" s="9"/>
       <c r="E518" s="9"/>
     </row>
-    <row r="519" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="519" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C519" s="9"/>
       <c r="E519" s="9"/>
     </row>
-    <row r="520" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="520" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C520" s="9"/>
       <c r="E520" s="9"/>
     </row>
-    <row r="521" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="521" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C521" s="9"/>
       <c r="E521" s="9"/>
     </row>
-    <row r="522" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="522" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C522" s="9"/>
       <c r="E522" s="9"/>
     </row>
-    <row r="523" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="523" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C523" s="9"/>
       <c r="E523" s="9"/>
     </row>
-    <row r="524" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="524" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C524" s="9"/>
       <c r="E524" s="9"/>
     </row>
-    <row r="525" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="525" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C525" s="9"/>
       <c r="E525" s="9"/>
     </row>
-    <row r="526" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="526" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C526" s="9"/>
       <c r="E526" s="9"/>
     </row>
-    <row r="527" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="527" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C527" s="9"/>
       <c r="E527" s="9"/>
     </row>
-    <row r="528" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="528" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C528" s="9"/>
       <c r="E528" s="9"/>
     </row>
-    <row r="529" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="529" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C529" s="9"/>
       <c r="E529" s="9"/>
     </row>
-    <row r="530" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="530" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C530" s="9"/>
       <c r="E530" s="9"/>
     </row>
-    <row r="531" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="531" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C531" s="9"/>
       <c r="E531" s="9"/>
     </row>
-    <row r="532" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="532" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C532" s="9"/>
       <c r="E532" s="9"/>
     </row>
-    <row r="533" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="533" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C533" s="9"/>
       <c r="E533" s="9"/>
     </row>
-    <row r="534" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="534" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C534" s="9"/>
       <c r="E534" s="9"/>
     </row>
-    <row r="535" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="535" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C535" s="9"/>
       <c r="E535" s="9"/>
     </row>
-    <row r="536" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="536" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C536" s="9"/>
       <c r="E536" s="9"/>
     </row>
-    <row r="537" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="537" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C537" s="9"/>
       <c r="E537" s="9"/>
     </row>
-    <row r="538" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="538" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C538" s="9"/>
       <c r="E538" s="9"/>
     </row>
-    <row r="539" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="539" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C539" s="9"/>
       <c r="E539" s="9"/>
     </row>
-    <row r="540" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="540" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C540" s="9"/>
       <c r="E540" s="9"/>
     </row>
-    <row r="541" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="541" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C541" s="9"/>
       <c r="E541" s="9"/>
     </row>
-    <row r="542" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="542" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C542" s="9"/>
       <c r="E542" s="9"/>
     </row>
-    <row r="543" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="543" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C543" s="9"/>
       <c r="E543" s="9"/>
     </row>
-    <row r="544" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="544" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C544" s="9"/>
       <c r="E544" s="9"/>
     </row>
-    <row r="545" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="545" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C545" s="9"/>
       <c r="E545" s="9"/>
     </row>
-    <row r="546" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="546" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C546" s="9"/>
       <c r="E546" s="9"/>
     </row>
-    <row r="547" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="547" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C547" s="9"/>
       <c r="E547" s="9"/>
     </row>
-    <row r="548" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="548" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C548" s="9"/>
       <c r="E548" s="9"/>
     </row>
-    <row r="549" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="549" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C549" s="9"/>
       <c r="E549" s="9"/>
     </row>
-    <row r="550" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="550" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C550" s="9"/>
       <c r="E550" s="9"/>
     </row>
-    <row r="551" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="551" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C551" s="9"/>
       <c r="E551" s="9"/>
     </row>
-    <row r="552" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="552" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C552" s="9"/>
       <c r="E552" s="9"/>
     </row>
-    <row r="553" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="553" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C553" s="9"/>
       <c r="E553" s="9"/>
     </row>
-    <row r="554" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="554" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C554" s="9"/>
       <c r="E554" s="9"/>
     </row>
-    <row r="555" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="555" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C555" s="9"/>
       <c r="E555" s="9"/>
     </row>
-    <row r="556" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="556" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C556" s="9"/>
       <c r="E556" s="9"/>
     </row>
-    <row r="557" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="557" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C557" s="9"/>
       <c r="E557" s="9"/>
     </row>
-    <row r="558" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="558" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C558" s="9"/>
       <c r="E558" s="9"/>
     </row>
-    <row r="559" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="559" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C559" s="9"/>
       <c r="E559" s="9"/>
     </row>
-    <row r="560" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="560" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C560" s="9"/>
       <c r="E560" s="9"/>
     </row>
-    <row r="561" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="561" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C561" s="9"/>
       <c r="E561" s="9"/>
     </row>
-    <row r="562" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="562" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C562" s="9"/>
       <c r="E562" s="9"/>
     </row>
-    <row r="563" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="563" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C563" s="9"/>
       <c r="E563" s="9"/>
     </row>
-    <row r="564" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="564" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C564" s="9"/>
       <c r="E564" s="9"/>
     </row>
-    <row r="565" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="565" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C565" s="9"/>
       <c r="E565" s="9"/>
     </row>
-    <row r="566" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="566" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C566" s="9"/>
       <c r="E566" s="9"/>
     </row>
-    <row r="567" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="567" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C567" s="9"/>
       <c r="E567" s="9"/>
     </row>
-    <row r="568" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="568" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C568" s="9"/>
       <c r="E568" s="9"/>
     </row>
-    <row r="569" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="569" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C569" s="9"/>
       <c r="E569" s="9"/>
     </row>
-    <row r="570" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="570" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C570" s="9"/>
       <c r="E570" s="9"/>
     </row>
-    <row r="571" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="571" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C571" s="9"/>
       <c r="E571" s="9"/>
     </row>
-    <row r="572" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="572" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C572" s="9"/>
       <c r="E572" s="9"/>
     </row>
-    <row r="573" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="573" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C573" s="9"/>
       <c r="E573" s="9"/>
     </row>
-    <row r="574" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="574" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C574" s="9"/>
       <c r="E574" s="9"/>
     </row>
-    <row r="575" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="575" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C575" s="9"/>
       <c r="E575" s="9"/>
     </row>
-    <row r="576" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="576" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C576" s="9"/>
       <c r="E576" s="9"/>
     </row>
-    <row r="577" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="577" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C577" s="9"/>
       <c r="E577" s="9"/>
     </row>
-    <row r="578" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="578" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C578" s="9"/>
       <c r="E578" s="9"/>
     </row>
-    <row r="579" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="579" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C579" s="9"/>
       <c r="E579" s="9"/>
     </row>
-    <row r="580" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="580" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C580" s="9"/>
       <c r="E580" s="9"/>
     </row>
-    <row r="581" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="581" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C581" s="9"/>
       <c r="E581" s="9"/>
     </row>
-    <row r="582" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="582" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C582" s="9"/>
       <c r="E582" s="9"/>
     </row>
-    <row r="583" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="583" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C583" s="9"/>
       <c r="E583" s="9"/>
     </row>
-    <row r="584" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="584" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C584" s="9"/>
       <c r="E584" s="9"/>
     </row>
-    <row r="585" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="585" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C585" s="9"/>
       <c r="E585" s="9"/>
     </row>

</xml_diff>

<commit_message>
Complete Acceptence Test Plan for Sprint 3.
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\water\Favorites\team-project-2245-swen-261-04-6f\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B584A442-6F91-4168-B75C-129066A3206C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C072E57C-59B5-4AEF-9BF0-936D7CF2BD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="53">
   <si>
     <t>Instructions</t>
   </si>
@@ -536,9 +536,6 @@
     <t>Given I change something as a user, when I log out then I expect my changes to be saved for when I log back in</t>
   </si>
   <si>
-    <t>not implemented yet</t>
-  </si>
-  <si>
     <t>As a Helper, I want to see a list of all available needs so that I can decide which ones to support.</t>
   </si>
   <si>
@@ -570,6 +567,9 @@
   </si>
   <si>
     <t>E.Z.W.; 04/07/2025;</t>
+  </si>
+  <si>
+    <t>A.M.; 04/07/2025</t>
   </si>
 </sst>
 </file>
@@ -1077,9 +1077,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F585"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C16" sqref="C16"/>
+      <selection pane="topRight" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1304,9 +1304,11 @@
       <c r="B16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="D16" s="4" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="E16" s="9"/>
     </row>
@@ -1318,7 +1320,7 @@
         <v>13</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" s="9"/>
     </row>
@@ -1330,7 +1332,7 @@
         <v>13</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E18" s="9"/>
     </row>
@@ -1345,90 +1347,100 @@
         <v>13</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="9"/>
+        <v>43</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="9"/>
+      <c r="C22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E26" s="9"/>
     </row>

</xml_diff>